<commit_message>
Sección 4.3.2.3.1.1 pendings completa
Signed-off-by: qa-katalon <qa-katalon@DEV-QA-KatalonStudio.BMinc.eu>
</commit_message>
<xml_diff>
--- a/Data Files/TestData/Reports/TestResults.xlsx
+++ b/Data Files/TestData/Reports/TestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\QAPregameNuevo\Data Files\TestData\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D28F93-6AC1-4D96-9EDC-E3ED1269B069}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B26A9B7-D1A6-41F6-BA12-A0AC16B5ED9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C6414" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,19 @@
     <sheet name="C3797" sheetId="12" r:id="rId10"/>
     <sheet name="C3860" sheetId="13" r:id="rId11"/>
     <sheet name="C3861" sheetId="15" r:id="rId12"/>
-    <sheet name="C3900" sheetId="14" r:id="rId13"/>
-    <sheet name="C3783" sheetId="6" r:id="rId14"/>
-    <sheet name="C3787" sheetId="7" r:id="rId15"/>
+    <sheet name="C3858" sheetId="16" r:id="rId13"/>
+    <sheet name="C3900" sheetId="14" r:id="rId14"/>
+    <sheet name="C3783" sheetId="6" r:id="rId15"/>
+    <sheet name="C3787" sheetId="7" r:id="rId16"/>
+    <sheet name="C3859" sheetId="17" r:id="rId17"/>
+    <sheet name="C3873" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="187">
   <si>
     <t>URL</t>
   </si>
@@ -87,9 +90,6 @@
     <t>http://pregame-support.bminc.eu</t>
   </si>
   <si>
-    <t>4fku01</t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
@@ -108,9 +108,6 @@
     <t>el formulario de ingreso es visible</t>
   </si>
   <si>
-    <t>El sistema no permitio que el usuario ingresará al sitio sin definir el pin de forma exitosa. El esperado mensaje de error 'The username or password is incorrect.' es desplegado existosamente</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>El sistema no permitio que el usuario ingresará al sitio con la tecla Enter si el PIN es incorrecto de forma exitosa. El esperado mensaje de error 'The username or password is incorrect.' es desplegado existosamente</t>
   </si>
   <si>
-    <t>SHA20012SHA20012</t>
-  </si>
-  <si>
     <t>10:25:03.255</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>El jugador no logró ingresar al sitio de pregame con la tecla enter, la pagina esperada debería tener el domino o sección sportbook pero actualmente es: http://www.jueguelo.com/home</t>
   </si>
   <si>
-    <t>http://10.0.74.5/index/home</t>
-  </si>
-  <si>
     <t>La opción de recordar credenciales es visible correctamente</t>
   </si>
   <si>
@@ -207,27 +198,6 @@
     <t>14:41:26.520</t>
   </si>
   <si>
-    <t>14:41:27.987</t>
-  </si>
-  <si>
-    <t>14:41:32.716</t>
-  </si>
-  <si>
-    <t>123456123456</t>
-  </si>
-  <si>
-    <t>14:41:35.331</t>
-  </si>
-  <si>
-    <t>14:41:41.897</t>
-  </si>
-  <si>
-    <t>14:41:44.604</t>
-  </si>
-  <si>
-    <t>14:41:49.487</t>
-  </si>
-  <si>
     <t>14:41:44.515</t>
   </si>
   <si>
@@ -237,9 +207,6 @@
     <t>Sistema Operativo</t>
   </si>
   <si>
-    <t>25/10/2019</t>
-  </si>
-  <si>
     <t>Permiso de Sportbook Sports es correctamente accesible para el usuario</t>
   </si>
   <si>
@@ -249,391 +216,388 @@
     <t>El botón login es visible</t>
   </si>
   <si>
-    <t>10:45:53.355</t>
-  </si>
-  <si>
-    <t>10:46:06.718</t>
-  </si>
-  <si>
-    <t>10:45:52.840</t>
-  </si>
-  <si>
-    <t>10:46:27.061</t>
-  </si>
-  <si>
-    <t>10:45:52.022</t>
-  </si>
-  <si>
-    <t>10:46:32.493</t>
-  </si>
-  <si>
-    <t>10:45:51.154</t>
-  </si>
-  <si>
-    <t>10:46:34.147</t>
-  </si>
-  <si>
-    <t>10:50:23.409</t>
-  </si>
-  <si>
-    <t>10:50:36.724</t>
-  </si>
-  <si>
-    <t>10:50:22.926</t>
-  </si>
-  <si>
-    <t>10:50:56.755</t>
-  </si>
-  <si>
-    <t>10:50:22.078</t>
-  </si>
-  <si>
-    <t>10:51:02.022</t>
-  </si>
-  <si>
-    <t>10:50:21.246</t>
-  </si>
-  <si>
-    <t>10:51:03.410</t>
-  </si>
-  <si>
-    <t>10:50:20.265</t>
-  </si>
-  <si>
-    <t>10:51:04.421</t>
-  </si>
-  <si>
-    <t>Los botones graded y pending de la sección de  reportes son visibles</t>
-  </si>
-  <si>
     <t>26/10/2019</t>
   </si>
   <si>
-    <t>09:20:58.859</t>
-  </si>
-  <si>
-    <t>09:21:13.016</t>
-  </si>
-  <si>
-    <t>09:20:58.420</t>
-  </si>
-  <si>
-    <t>09:21:23.548</t>
-  </si>
-  <si>
-    <t>09:20:57.636</t>
-  </si>
-  <si>
-    <t>09:21:28.580</t>
-  </si>
-  <si>
-    <t>09:20:56.848</t>
-  </si>
-  <si>
-    <t>09:21:29.880</t>
-  </si>
-  <si>
-    <t>09:20:26.704</t>
-  </si>
-  <si>
-    <t>09:21:30.679</t>
-  </si>
-  <si>
-    <t>10:42:44.708</t>
-  </si>
-  <si>
-    <t>10:43:12.374</t>
-  </si>
-  <si>
-    <t>El botón de reportes de la sección "My Account no es visible debido a un error anomalo en la prueba. Favor revisar los log o bitacoras de katalon</t>
-  </si>
-  <si>
-    <t>10:47:43.761</t>
-  </si>
-  <si>
-    <t>10:48:14.933</t>
-  </si>
-  <si>
-    <t>10:47:42.965</t>
-  </si>
-  <si>
-    <t>10:48:25.011</t>
-  </si>
-  <si>
-    <t>10:47:41.780</t>
-  </si>
-  <si>
-    <t>10:48:53.618</t>
-  </si>
-  <si>
-    <t>10:47:40.657</t>
-  </si>
-  <si>
-    <t>10:48:55.079</t>
-  </si>
-  <si>
-    <t>10:46:58.806</t>
-  </si>
-  <si>
-    <t>10:48:56.186</t>
-  </si>
-  <si>
-    <t>El botón graded o pending  no esta visible despues de presionar el botón de Reportes. Favor revisar las tomas instantaneas</t>
-  </si>
-  <si>
-    <t>10:52:03.347</t>
-  </si>
-  <si>
-    <t>10:52:16.773</t>
-  </si>
-  <si>
-    <t>10:52:02.880</t>
-  </si>
-  <si>
-    <t>10:52:26.914</t>
-  </si>
-  <si>
-    <t>10:52:02.238</t>
-  </si>
-  <si>
-    <t>10:52:32.001</t>
-  </si>
-  <si>
-    <t>10:52:01.570</t>
-  </si>
-  <si>
-    <t>10:52:33.307</t>
-  </si>
-  <si>
-    <t>10:51:32.868</t>
-  </si>
-  <si>
-    <t>10:52:34.122</t>
-  </si>
-  <si>
-    <t>10:55:37.398</t>
-  </si>
-  <si>
-    <t>10:55:50.006</t>
-  </si>
-  <si>
-    <t>10:55:36.683</t>
-  </si>
-  <si>
-    <t>10:56:00.288</t>
-  </si>
-  <si>
-    <t>10:55:35.582</t>
-  </si>
-  <si>
-    <t>10:56:05.663</t>
-  </si>
-  <si>
-    <t>10:55:34.469</t>
-  </si>
-  <si>
-    <t>10:56:07.160</t>
-  </si>
-  <si>
-    <t>10:57:48.564</t>
-  </si>
-  <si>
-    <t>10:58:03.601</t>
-  </si>
-  <si>
-    <t>10:57:48.096</t>
-  </si>
-  <si>
-    <t>10:58:13.682</t>
-  </si>
-  <si>
-    <t>10:57:47.400</t>
-  </si>
-  <si>
-    <t>10:58:18.792</t>
-  </si>
-  <si>
-    <t>10:57:46.678</t>
-  </si>
-  <si>
-    <t>10:58:20.057</t>
-  </si>
-  <si>
-    <t>10:57:18.444</t>
-  </si>
-  <si>
-    <t>10:58:21.218</t>
-  </si>
-  <si>
-    <t>10:59:48.920</t>
-  </si>
-  <si>
-    <t>11:00:02.677</t>
-  </si>
-  <si>
-    <t>10:59:48.462</t>
-  </si>
-  <si>
-    <t>11:00:12.662</t>
-  </si>
-  <si>
-    <t>10:59:47.724</t>
-  </si>
-  <si>
-    <t>11:00:17.863</t>
-  </si>
-  <si>
-    <t>10:59:47.006</t>
-  </si>
-  <si>
-    <t>11:00:19.231</t>
-  </si>
-  <si>
-    <t>10:59:17.415</t>
-  </si>
-  <si>
-    <t>11:00:20.396</t>
-  </si>
-  <si>
-    <t>11:01:41.568</t>
-  </si>
-  <si>
-    <t>11:01:55.701</t>
-  </si>
-  <si>
-    <t>11:01:40.773</t>
-  </si>
-  <si>
-    <t>11:02:05.918</t>
-  </si>
-  <si>
-    <t>11:01:39.597</t>
-  </si>
-  <si>
-    <t>11:02:11.139</t>
-  </si>
-  <si>
-    <t>11:01:38.548</t>
-  </si>
-  <si>
-    <t>11:02:12.772</t>
-  </si>
-  <si>
-    <t>11:03:27.808</t>
-  </si>
-  <si>
-    <t>11:03:42.283</t>
-  </si>
-  <si>
-    <t>11:03:27.182</t>
-  </si>
-  <si>
-    <t>11:03:52.243</t>
-  </si>
-  <si>
-    <t>11:03:26.001</t>
-  </si>
-  <si>
-    <t>11:03:57.363</t>
-  </si>
-  <si>
-    <t>11:03:24.969</t>
-  </si>
-  <si>
-    <t>11:03:58.915</t>
-  </si>
-  <si>
-    <t>11:05:14.192</t>
-  </si>
-  <si>
-    <t>11:05:29.324</t>
-  </si>
-  <si>
-    <t>11:05:13.471</t>
-  </si>
-  <si>
-    <t>11:05:39.234</t>
-  </si>
-  <si>
-    <t>11:05:12.383</t>
-  </si>
-  <si>
-    <t>11:05:44.483</t>
-  </si>
-  <si>
-    <t>11:05:11.327</t>
-  </si>
-  <si>
-    <t>11:05:46.086</t>
-  </si>
-  <si>
-    <t>11:04:41.345</t>
-  </si>
-  <si>
-    <t>11:06:39.345</t>
-  </si>
-  <si>
-    <t>11:31:10.105</t>
-  </si>
-  <si>
-    <t>11:31:29.428</t>
-  </si>
-  <si>
-    <t>11:31:09.601</t>
-  </si>
-  <si>
-    <t>11:31:40.841</t>
-  </si>
-  <si>
-    <t>11:31:08.787</t>
-  </si>
-  <si>
-    <t>11:31:46.191</t>
-  </si>
-  <si>
-    <t>11:31:07.410</t>
-  </si>
-  <si>
-    <t>11:31:47.606</t>
-  </si>
-  <si>
-    <t>11:30:37.518</t>
-  </si>
-  <si>
-    <t>11:31:48.519</t>
-  </si>
-  <si>
-    <t>El botón  pending  no está seleccionado de forma predeterminada al presionar el botón account o, las apuestas pendientes de customer maintenance no se reflejan correctamente en pregame. Si se desea, se puede revisar en el log dfe katalon con el código -10</t>
-  </si>
-  <si>
-    <t>11:34:30.081</t>
-  </si>
-  <si>
-    <t>11:34:48.332</t>
-  </si>
-  <si>
-    <t>11:34:29.649</t>
-  </si>
-  <si>
-    <t>11:34:59.113</t>
-  </si>
-  <si>
-    <t>11:34:28.802</t>
-  </si>
-  <si>
-    <t>11:35:04.631</t>
-  </si>
-  <si>
-    <t>11:34:28.066</t>
-  </si>
-  <si>
-    <t>11:35:05.992</t>
-  </si>
-  <si>
-    <t>11:33:55.715</t>
-  </si>
-  <si>
-    <t>11:35:07.150</t>
+    <t>El mensaje de error esperado debería ser The username or password is incorrect. pero actualmente es: The username or password is incorrect. .Sio se desea, se puede ver la traza de este error con el siguiente código -10</t>
+  </si>
+  <si>
+    <t>14:24:00.789</t>
+  </si>
+  <si>
+    <t>14:24:23.231</t>
+  </si>
+  <si>
+    <t>28/10/2019</t>
+  </si>
+  <si>
+    <t>08:49:48.682</t>
+  </si>
+  <si>
+    <t>08:50:06.553</t>
+  </si>
+  <si>
+    <t>08:49:47.787</t>
+  </si>
+  <si>
+    <t>08:50:09.556</t>
+  </si>
+  <si>
+    <t>El botón pending aparece seleccionado de forma predeterminada correctamente</t>
+  </si>
+  <si>
+    <t>El boton de pending se ve correctamente</t>
+  </si>
+  <si>
+    <t>31/10/2019</t>
+  </si>
+  <si>
+    <t>4FKU01</t>
+  </si>
+  <si>
+    <t>11:07:07.612</t>
+  </si>
+  <si>
+    <t>11:07:11.675</t>
+  </si>
+  <si>
+    <t>11:07:07.153</t>
+  </si>
+  <si>
+    <t>11:07:22.075</t>
+  </si>
+  <si>
+    <t>11:07:06.381</t>
+  </si>
+  <si>
+    <t>11:07:27.062</t>
+  </si>
+  <si>
+    <t>11:07:05.608</t>
+  </si>
+  <si>
+    <t>11:07:28.342</t>
+  </si>
+  <si>
+    <t>11:07:04.965</t>
+  </si>
+  <si>
+    <t>11:07:29.178</t>
+  </si>
+  <si>
+    <t>11:07:04.289</t>
+  </si>
+  <si>
+    <t>11:07:32.085</t>
+  </si>
+  <si>
+    <t>11:06:36.212</t>
+  </si>
+  <si>
+    <t>11:07:34.608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las apuestas 151957379-1,151957378-1  del jugador 4FKU01 aparecen correctamente en la sección Pensdings de reprotes </t>
+  </si>
+  <si>
+    <t>12:01:42.195</t>
+  </si>
+  <si>
+    <t>12:02:09.641</t>
+  </si>
+  <si>
+    <t>La prueba resulto fallida porque el jugador de prueba  tiene apuestas pendientes en customer maintenance, o algún componente que no pudó ser localizado.  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>12:04:13.477</t>
+  </si>
+  <si>
+    <t>12:04:17.145</t>
+  </si>
+  <si>
+    <t>4FKU09</t>
+  </si>
+  <si>
+    <t>12:04:13.016</t>
+  </si>
+  <si>
+    <t>12:04:27.158</t>
+  </si>
+  <si>
+    <t>12:04:12.171</t>
+  </si>
+  <si>
+    <t>12:04:32.307</t>
+  </si>
+  <si>
+    <t>12:04:11.563</t>
+  </si>
+  <si>
+    <t>12:04:33.680</t>
+  </si>
+  <si>
+    <t>12:04:10.953</t>
+  </si>
+  <si>
+    <t>12:04:34.525</t>
+  </si>
+  <si>
+    <t>12:04:10.251</t>
+  </si>
+  <si>
+    <t>12:04:37.649</t>
+  </si>
+  <si>
+    <t>12:03:44.184</t>
+  </si>
+  <si>
+    <t>12:04:39.120</t>
+  </si>
+  <si>
+    <t>13:08:40.486</t>
+  </si>
+  <si>
+    <t>13:08:43.843</t>
+  </si>
+  <si>
+    <t>13:08:40.052</t>
+  </si>
+  <si>
+    <t>13:08:53.998</t>
+  </si>
+  <si>
+    <t>13:08:39.335</t>
+  </si>
+  <si>
+    <t>13:08:59.050</t>
+  </si>
+  <si>
+    <t>13:08:38.642</t>
+  </si>
+  <si>
+    <t>13:09:00.478</t>
+  </si>
+  <si>
+    <t>13:08:38.036</t>
+  </si>
+  <si>
+    <t>13:09:01.310</t>
+  </si>
+  <si>
+    <t>13:08:37.372</t>
+  </si>
+  <si>
+    <t>13:09:04.213</t>
+  </si>
+  <si>
+    <t>13:08:11.851</t>
+  </si>
+  <si>
+    <t>13:09:05.988</t>
+  </si>
+  <si>
+    <t>13:34:14.901</t>
+  </si>
+  <si>
+    <t>13:36:23.245</t>
+  </si>
+  <si>
+    <t>13:42:12.189</t>
+  </si>
+  <si>
+    <t>13:42:15.662</t>
+  </si>
+  <si>
+    <t>13:42:11.760</t>
+  </si>
+  <si>
+    <t>13:42:25.982</t>
+  </si>
+  <si>
+    <t>13:42:10.960</t>
+  </si>
+  <si>
+    <t>13:42:31.073</t>
+  </si>
+  <si>
+    <t>13:42:10.243</t>
+  </si>
+  <si>
+    <t>13:42:32.419</t>
+  </si>
+  <si>
+    <t>13:42:09.681</t>
+  </si>
+  <si>
+    <t>13:42:33.424</t>
+  </si>
+  <si>
+    <t>13:42:09.117</t>
+  </si>
+  <si>
+    <t>13:42:36.397</t>
+  </si>
+  <si>
+    <t>13:41:38.186</t>
+  </si>
+  <si>
+    <t>13:43:09.039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las apuestas 149759472-1,149171605-1,149168598-1,148870322-1,148044827-1,147749161-1,147411523-1,147369582-1,147369542-1,139379305-1,139253058-1,126684928-1,126684926-1,126684332-1,126684331-1,126684207-1,126684206-1,126684181-1,126684181-2,126684181-3,126679558-1,126606266-1,126599972-1,126597438-1,126588880-1,126587026-1,126587021-1,126561493-1,126561492-1,126560710-1,126560532-1,126560529-1,126560527-1,126560504-1,126559586-1,126559219-1,126559173-1,126558027-1  del jugador 4FKU09 aparecen correctamente en la sección Pensdings de reprotes </t>
+  </si>
+  <si>
+    <t>4FKU100</t>
+  </si>
+  <si>
+    <t>13:49:16.261</t>
+  </si>
+  <si>
+    <t>13:50:13.581</t>
+  </si>
+  <si>
+    <t>La prueba resulto fallida por algún fallo anomalo. Favor de revisar en la consola de katalon con el siguiente código -99</t>
+  </si>
+  <si>
+    <t>14:07:11.393</t>
+  </si>
+  <si>
+    <t>14:08:08.776</t>
+  </si>
+  <si>
+    <t>14:12:15.062</t>
+  </si>
+  <si>
+    <t>14:12:52.472</t>
+  </si>
+  <si>
+    <t>14:18:19.688</t>
+  </si>
+  <si>
+    <t>14:18:22.737</t>
+  </si>
+  <si>
+    <t>14:18:19.188</t>
+  </si>
+  <si>
+    <t>14:18:32.662</t>
+  </si>
+  <si>
+    <t>14:18:18.459</t>
+  </si>
+  <si>
+    <t>14:18:37.756</t>
+  </si>
+  <si>
+    <t>14:18:17.802</t>
+  </si>
+  <si>
+    <t>14:18:39.055</t>
+  </si>
+  <si>
+    <t>14:18:17.292</t>
+  </si>
+  <si>
+    <t>14:18:39.802</t>
+  </si>
+  <si>
+    <t>14:18:16.740</t>
+  </si>
+  <si>
+    <t>14:18:42.643</t>
+  </si>
+  <si>
+    <t>14:17:38.569</t>
+  </si>
+  <si>
+    <t>14:18:47.118</t>
+  </si>
+  <si>
+    <t>14:20:19.716</t>
+  </si>
+  <si>
+    <t>14:20:22.918</t>
+  </si>
+  <si>
+    <t>14:20:19.275</t>
+  </si>
+  <si>
+    <t>14:20:32.618</t>
+  </si>
+  <si>
+    <t>14:20:18.521</t>
+  </si>
+  <si>
+    <t>14:20:37.856</t>
+  </si>
+  <si>
+    <t>14:20:17.825</t>
+  </si>
+  <si>
+    <t>14:20:39.195</t>
+  </si>
+  <si>
+    <t>14:20:17.191</t>
+  </si>
+  <si>
+    <t>14:20:39.961</t>
+  </si>
+  <si>
+    <t>14:20:16.452</t>
+  </si>
+  <si>
+    <t>14:20:42.865</t>
+  </si>
+  <si>
+    <t>14:19:38.523</t>
+  </si>
+  <si>
+    <t>14:20:53.316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El botón de pendings muestra existosamente que el 4FKU100 no tiene apuestas pendientes </t>
+  </si>
+  <si>
+    <t>14:37:11.447</t>
+  </si>
+  <si>
+    <t>14:37:35.019</t>
+  </si>
+  <si>
+    <t>14:37:10.813</t>
+  </si>
+  <si>
+    <t>14:37:44.857</t>
+  </si>
+  <si>
+    <t>14:37:09.795</t>
+  </si>
+  <si>
+    <t>14:38:00.536</t>
+  </si>
+  <si>
+    <t>14:37:08.851</t>
+  </si>
+  <si>
+    <t>14:38:02.156</t>
+  </si>
+  <si>
+    <t>14:37:07.888</t>
+  </si>
+  <si>
+    <t>14:38:03.042</t>
+  </si>
+  <si>
+    <t>14:37:06.914</t>
+  </si>
+  <si>
+    <t>14:38:06.018</t>
+  </si>
+  <si>
+    <t>14:35:54.952</t>
+  </si>
+  <si>
+    <t>14:38:26.831</t>
   </si>
 </sst>
 </file>
@@ -1066,25 +1030,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1149,28 +1113,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1179,7 +1143,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1217,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1237,25 +1201,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="F2" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1264,7 +1228,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1274,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42775E94-9CE9-4EF9-979B-7209E1E7B720}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,7 +1277,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1328,30 +1292,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="F2" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1360,7 +1324,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1369,11 +1333,103 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747D2F54-78BA-4A51-916E-7AC9EBC20560}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612D7C13-804A-4327-9778-778A01BF38DD}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:K1"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,7 +1463,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1427,25 +1483,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1454,7 +1510,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1462,7 +1518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1487,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1516,19 +1572,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -1537,7 +1593,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1545,13 +1601,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1563,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1592,19 +1646,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -1613,7 +1667,218 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381977F2-0229-4BC8-A029-42944E0535BF}">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" t="s">
+        <v>9</v>
+      </c>
+      <c r="J43" t="s">
+        <v>10</v>
+      </c>
+      <c r="K43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3043AB7-CB0A-4C57-8B73-07EA10FF0C55}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1683,25 +1948,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1710,7 +1975,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1781,37 +2046,37 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1872,37 +2137,37 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1965,25 +2230,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1992,7 +2257,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2054,25 +2319,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2081,7 +2346,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2139,25 +2404,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2166,7 +2431,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2226,25 +2491,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2253,7 +2518,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -2302,22 +2567,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -2326,7 +2591,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inclusión de daily Fgigure
Signed-off-by: qa-katalon <qa-katalon@DEV-QA-KatalonStudio.BMinc.eu>
</commit_message>
<xml_diff>
--- a/Data Files/TestData/Reports/TestResults.xlsx
+++ b/Data Files/TestData/Reports/TestResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\QAPregameNuevo\Data Files\TestData\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B26A9B7-D1A6-41F6-BA12-A0AC16B5ED9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8083ECBB-9042-4716-84FF-BFC282DF6148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1845" windowWidth="21600" windowHeight="11385" firstSheet="15" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C6414" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,22 @@
     <sheet name="C3787" sheetId="7" r:id="rId16"/>
     <sheet name="C3859" sheetId="17" r:id="rId17"/>
     <sheet name="C3873" sheetId="18" r:id="rId18"/>
+    <sheet name="C3870" sheetId="19" r:id="rId19"/>
+    <sheet name="C3874" sheetId="20" r:id="rId20"/>
+    <sheet name="C6397" sheetId="22" r:id="rId21"/>
+    <sheet name="C3864" sheetId="23" r:id="rId22"/>
+    <sheet name="C6398" sheetId="24" r:id="rId23"/>
+    <sheet name="C3876" sheetId="25" r:id="rId24"/>
+    <sheet name="C6399" sheetId="26" r:id="rId25"/>
+    <sheet name="C6400" sheetId="27" r:id="rId26"/>
+    <sheet name="C3875" sheetId="21" r:id="rId27"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="402">
   <si>
     <t>URL</t>
   </si>
@@ -105,9 +114,6 @@
     <t>Fecha de prueba</t>
   </si>
   <si>
-    <t>el formulario de ingreso es visible</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -153,451 +159,1099 @@
     <t>La opción de recordar credenciales es visible correctamente</t>
   </si>
   <si>
-    <t>23/10/2019</t>
-  </si>
-  <si>
     <t>La función de recordar credenciales  funciona correctamente</t>
   </si>
   <si>
-    <t>1930</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>10:49:09.767</t>
-  </si>
-  <si>
-    <t>10:49:30.495</t>
-  </si>
-  <si>
-    <t>10:49:08.830</t>
-  </si>
-  <si>
-    <t>10:49:56.599</t>
-  </si>
-  <si>
     <t>El sistema no permitio que el usuario ingresará al sitio si la clave no es ingresada de forma exitosa. El esperado mensaje de error 'The username or password is incorrect.' es desplegado existosamente</t>
   </si>
   <si>
-    <t>14:40:54.272</t>
-  </si>
-  <si>
-    <t>14:41:15.896</t>
-  </si>
-  <si>
-    <t>14:41:17.735</t>
-  </si>
-  <si>
-    <t>14:41:21.552</t>
-  </si>
-  <si>
-    <t>14:41:22.948</t>
-  </si>
-  <si>
-    <t>14:41:26.520</t>
-  </si>
-  <si>
-    <t>14:41:44.515</t>
-  </si>
-  <si>
-    <t>14:41:51.514</t>
-  </si>
-  <si>
     <t>Sistema Operativo</t>
   </si>
   <si>
+    <t>El botón de reportes de la sección "My Account" es visible</t>
+  </si>
+  <si>
+    <t>El botón login es visible</t>
+  </si>
+  <si>
+    <t>El botón pending aparece seleccionado de forma predeterminada correctamente</t>
+  </si>
+  <si>
+    <t>El boton de pending se ve correctamente</t>
+  </si>
+  <si>
+    <t>http://10.0.74.5/index/home</t>
+  </si>
+  <si>
+    <t>01/11/2019</t>
+  </si>
+  <si>
+    <t>4FKU01</t>
+  </si>
+  <si>
+    <t>10:26:02.579</t>
+  </si>
+  <si>
+    <t>10:27:21.291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El botón de pendings muestra existosamente que el jugador 4FKU01 no tiene apuestas pendientes </t>
+  </si>
+  <si>
+    <t>-HOE115</t>
+  </si>
+  <si>
+    <t>Ksvwbnk9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las apuestas 174739697-1,174739592-1,174739449-1  del jugador -HOE115 aparecen correctamente en la sección Pensdings de reprotes </t>
+  </si>
+  <si>
+    <t>-RI137</t>
+  </si>
+  <si>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>14:12:21.294</t>
+  </si>
+  <si>
+    <t>14:14:20.931</t>
+  </si>
+  <si>
+    <t>La prueba resulto fallida porque el jugador de prueba no tiene apuestas resueltas en customer maintenance, o algún componente que no pudó ser localizado.  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>15:00:56.135</t>
+  </si>
+  <si>
+    <t>15:01:30.571</t>
+  </si>
+  <si>
+    <t>15:00:55.444</t>
+  </si>
+  <si>
+    <t>15:01:33.558</t>
+  </si>
+  <si>
+    <t>15:00:27.986</t>
+  </si>
+  <si>
+    <t>15:01:36.339</t>
+  </si>
+  <si>
+    <t>4FKU100</t>
+  </si>
+  <si>
+    <t>15:44:46.030</t>
+  </si>
+  <si>
+    <t>15:45:07.526</t>
+  </si>
+  <si>
+    <t>15:44:45.367</t>
+  </si>
+  <si>
+    <t>15:45:08.566</t>
+  </si>
+  <si>
+    <t>Botón Graded es visible de forma satisfactoria</t>
+  </si>
+  <si>
+    <t>15:44:08.127</t>
+  </si>
+  <si>
+    <t>15:45:12.420</t>
+  </si>
+  <si>
+    <t>El sitio de pregame no muestra apuestas resueltas  del jugador 4FKU100 de forma exitosa</t>
+  </si>
+  <si>
+    <t>04/11/2019</t>
+  </si>
+  <si>
+    <t>El sistema no permitio que el usuario ingresará al sitio sin definir el pin de forma exitosa. El esperado mensaje de error 'The username or password is incorrect.' es desplegado existosamente</t>
+  </si>
+  <si>
+    <t>09:24:15.985</t>
+  </si>
+  <si>
+    <t>09:24:36.700</t>
+  </si>
+  <si>
+    <t>09:24:38.273</t>
+  </si>
+  <si>
+    <t>09:24:42.110</t>
+  </si>
+  <si>
+    <t>09:24:43.490</t>
+  </si>
+  <si>
+    <t>09:24:46.862</t>
+  </si>
+  <si>
+    <t>09:24:48.334</t>
+  </si>
+  <si>
+    <t>09:24:57.023</t>
+  </si>
+  <si>
+    <t>09:24:58.477</t>
+  </si>
+  <si>
+    <t>09:25:08.285</t>
+  </si>
+  <si>
+    <t>09:25:11.769</t>
+  </si>
+  <si>
+    <t>09:25:19.551</t>
+  </si>
+  <si>
+    <t>09:25:23.667</t>
+  </si>
+  <si>
+    <t>09:25:28.836</t>
+  </si>
+  <si>
+    <t>09:25:23.585</t>
+  </si>
+  <si>
+    <t>09:25:30.812</t>
+  </si>
+  <si>
+    <t>09:25:23.062</t>
+  </si>
+  <si>
+    <t>09:25:51.563</t>
+  </si>
+  <si>
+    <t>El botón Daily Figure o Balance Diario de la sección "My Account" es visible</t>
+  </si>
+  <si>
+    <t>El combobox de semanas es visible</t>
+  </si>
+  <si>
+    <t>Chrome 78.0.3904.70</t>
+  </si>
+  <si>
+    <t>13:46:24.421</t>
+  </si>
+  <si>
+    <t>13:47:00.979</t>
+  </si>
+  <si>
+    <t>05/11/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El checkbox "Start From Tuesday" es visible correctamente </t>
+  </si>
+  <si>
+    <t>13:28:33.898</t>
+  </si>
+  <si>
+    <t>13:29:12.316</t>
+  </si>
+  <si>
+    <t>08/11/2019</t>
+  </si>
+  <si>
+    <t>12:28:27.066</t>
+  </si>
+  <si>
+    <t>12:29:03.954</t>
+  </si>
+  <si>
+    <t>Chrome 78.0.3904.87</t>
+  </si>
+  <si>
+    <t>12:28:26.341</t>
+  </si>
+  <si>
+    <t>12:29:18.644</t>
+  </si>
+  <si>
+    <t>12:28:25.352</t>
+  </si>
+  <si>
+    <t>12:29:41.876</t>
+  </si>
+  <si>
+    <t>Permiso de Sportbook Deportes es correctamente accesible para el usuario</t>
+  </si>
+  <si>
+    <t>12:28:24.262</t>
+  </si>
+  <si>
+    <t>12:29:43.705</t>
+  </si>
+  <si>
+    <t>12:28:23.254</t>
+  </si>
+  <si>
+    <t>12:29:49.844</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los días de la semana Lunes,Martes,Miércoles,Jueves,Viernes,Sábado,Domingo y  encabezado de sumatorial Total se ven correctamente en la tabla de días de la semana </t>
+  </si>
+  <si>
+    <t>12:28:21.855</t>
+  </si>
+  <si>
+    <t>12:30:09.189</t>
+  </si>
+  <si>
+    <t>El checkbox "Iniciar Martes" muestra correctamente los días de la semana con el siguiente orden: Martes,Miércoles,Jueves,Viernes,Sábado,Domingo,Lunes,Total</t>
+  </si>
+  <si>
+    <t>12:33:40.972</t>
+  </si>
+  <si>
+    <t>El jugador SHA2001 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes</t>
+  </si>
+  <si>
+    <t>PRAC06</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>12:36:33.823</t>
+  </si>
+  <si>
+    <t>El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes</t>
+  </si>
+  <si>
+    <t>12:38:18.484</t>
+  </si>
+  <si>
+    <t>12:46:10.742</t>
+  </si>
+  <si>
+    <t>13:18:36.791</t>
+  </si>
+  <si>
+    <t>13:18:39.738</t>
+  </si>
+  <si>
+    <t>13:18:36.120</t>
+  </si>
+  <si>
+    <t>13:18:52.047</t>
+  </si>
+  <si>
+    <t>13:18:34.964</t>
+  </si>
+  <si>
+    <t>13:18:59.900</t>
+  </si>
+  <si>
     <t>Permiso de Sportbook Sports es correctamente accesible para el usuario</t>
   </si>
   <si>
-    <t>El botón de reportes de la sección "My Account" es visible</t>
-  </si>
-  <si>
-    <t>El botón login es visible</t>
-  </si>
-  <si>
-    <t>26/10/2019</t>
-  </si>
-  <si>
-    <t>El mensaje de error esperado debería ser The username or password is incorrect. pero actualmente es: The username or password is incorrect. .Sio se desea, se puede ver la traza de este error con el siguiente código -10</t>
-  </si>
-  <si>
-    <t>14:24:00.789</t>
-  </si>
-  <si>
-    <t>14:24:23.231</t>
-  </si>
-  <si>
-    <t>28/10/2019</t>
-  </si>
-  <si>
-    <t>08:49:48.682</t>
-  </si>
-  <si>
-    <t>08:50:06.553</t>
-  </si>
-  <si>
-    <t>08:49:47.787</t>
-  </si>
-  <si>
-    <t>08:50:09.556</t>
-  </si>
-  <si>
-    <t>El botón pending aparece seleccionado de forma predeterminada correctamente</t>
-  </si>
-  <si>
-    <t>El boton de pending se ve correctamente</t>
-  </si>
-  <si>
-    <t>31/10/2019</t>
-  </si>
-  <si>
-    <t>4FKU01</t>
-  </si>
-  <si>
-    <t>11:07:07.612</t>
-  </si>
-  <si>
-    <t>11:07:11.675</t>
-  </si>
-  <si>
-    <t>11:07:07.153</t>
-  </si>
-  <si>
-    <t>11:07:22.075</t>
-  </si>
-  <si>
-    <t>11:07:06.381</t>
-  </si>
-  <si>
-    <t>11:07:27.062</t>
-  </si>
-  <si>
-    <t>11:07:05.608</t>
-  </si>
-  <si>
-    <t>11:07:28.342</t>
-  </si>
-  <si>
-    <t>11:07:04.965</t>
-  </si>
-  <si>
-    <t>11:07:29.178</t>
-  </si>
-  <si>
-    <t>11:07:04.289</t>
-  </si>
-  <si>
-    <t>11:07:32.085</t>
-  </si>
-  <si>
-    <t>11:06:36.212</t>
-  </si>
-  <si>
-    <t>11:07:34.608</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las apuestas 151957379-1,151957378-1  del jugador 4FKU01 aparecen correctamente en la sección Pensdings de reprotes </t>
-  </si>
-  <si>
-    <t>12:01:42.195</t>
-  </si>
-  <si>
-    <t>12:02:09.641</t>
-  </si>
-  <si>
-    <t>La prueba resulto fallida porque el jugador de prueba  tiene apuestas pendientes en customer maintenance, o algún componente que no pudó ser localizado.  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
-  </si>
-  <si>
-    <t>12:04:13.477</t>
-  </si>
-  <si>
-    <t>12:04:17.145</t>
-  </si>
-  <si>
-    <t>4FKU09</t>
-  </si>
-  <si>
-    <t>12:04:13.016</t>
-  </si>
-  <si>
-    <t>12:04:27.158</t>
-  </si>
-  <si>
-    <t>12:04:12.171</t>
-  </si>
-  <si>
-    <t>12:04:32.307</t>
-  </si>
-  <si>
-    <t>12:04:11.563</t>
-  </si>
-  <si>
-    <t>12:04:33.680</t>
-  </si>
-  <si>
-    <t>12:04:10.953</t>
-  </si>
-  <si>
-    <t>12:04:34.525</t>
-  </si>
-  <si>
-    <t>12:04:10.251</t>
-  </si>
-  <si>
-    <t>12:04:37.649</t>
-  </si>
-  <si>
-    <t>12:03:44.184</t>
-  </si>
-  <si>
-    <t>12:04:39.120</t>
-  </si>
-  <si>
-    <t>13:08:40.486</t>
-  </si>
-  <si>
-    <t>13:08:43.843</t>
-  </si>
-  <si>
-    <t>13:08:40.052</t>
-  </si>
-  <si>
-    <t>13:08:53.998</t>
-  </si>
-  <si>
-    <t>13:08:39.335</t>
-  </si>
-  <si>
-    <t>13:08:59.050</t>
-  </si>
-  <si>
-    <t>13:08:38.642</t>
-  </si>
-  <si>
-    <t>13:09:00.478</t>
-  </si>
-  <si>
-    <t>13:08:38.036</t>
-  </si>
-  <si>
-    <t>13:09:01.310</t>
-  </si>
-  <si>
-    <t>13:08:37.372</t>
-  </si>
-  <si>
-    <t>13:09:04.213</t>
-  </si>
-  <si>
-    <t>13:08:11.851</t>
-  </si>
-  <si>
-    <t>13:09:05.988</t>
-  </si>
-  <si>
-    <t>13:34:14.901</t>
-  </si>
-  <si>
-    <t>13:36:23.245</t>
-  </si>
-  <si>
-    <t>13:42:12.189</t>
-  </si>
-  <si>
-    <t>13:42:15.662</t>
-  </si>
-  <si>
-    <t>13:42:11.760</t>
-  </si>
-  <si>
-    <t>13:42:25.982</t>
-  </si>
-  <si>
-    <t>13:42:10.960</t>
-  </si>
-  <si>
-    <t>13:42:31.073</t>
-  </si>
-  <si>
-    <t>13:42:10.243</t>
-  </si>
-  <si>
-    <t>13:42:32.419</t>
-  </si>
-  <si>
-    <t>13:42:09.681</t>
-  </si>
-  <si>
-    <t>13:42:33.424</t>
-  </si>
-  <si>
-    <t>13:42:09.117</t>
-  </si>
-  <si>
-    <t>13:42:36.397</t>
-  </si>
-  <si>
-    <t>13:41:38.186</t>
-  </si>
-  <si>
-    <t>13:43:09.039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las apuestas 149759472-1,149171605-1,149168598-1,148870322-1,148044827-1,147749161-1,147411523-1,147369582-1,147369542-1,139379305-1,139253058-1,126684928-1,126684926-1,126684332-1,126684331-1,126684207-1,126684206-1,126684181-1,126684181-2,126684181-3,126679558-1,126606266-1,126599972-1,126597438-1,126588880-1,126587026-1,126587021-1,126561493-1,126561492-1,126560710-1,126560532-1,126560529-1,126560527-1,126560504-1,126559586-1,126559219-1,126559173-1,126558027-1  del jugador 4FKU09 aparecen correctamente en la sección Pensdings de reprotes </t>
-  </si>
-  <si>
-    <t>4FKU100</t>
-  </si>
-  <si>
-    <t>13:49:16.261</t>
-  </si>
-  <si>
-    <t>13:50:13.581</t>
-  </si>
-  <si>
-    <t>La prueba resulto fallida por algún fallo anomalo. Favor de revisar en la consola de katalon con el siguiente código -99</t>
-  </si>
-  <si>
-    <t>14:07:11.393</t>
-  </si>
-  <si>
-    <t>14:08:08.776</t>
-  </si>
-  <si>
-    <t>14:12:15.062</t>
-  </si>
-  <si>
-    <t>14:12:52.472</t>
-  </si>
-  <si>
-    <t>14:18:19.688</t>
-  </si>
-  <si>
-    <t>14:18:22.737</t>
-  </si>
-  <si>
-    <t>14:18:19.188</t>
-  </si>
-  <si>
-    <t>14:18:32.662</t>
-  </si>
-  <si>
-    <t>14:18:18.459</t>
-  </si>
-  <si>
-    <t>14:18:37.756</t>
-  </si>
-  <si>
-    <t>14:18:17.802</t>
-  </si>
-  <si>
-    <t>14:18:39.055</t>
-  </si>
-  <si>
-    <t>14:18:17.292</t>
-  </si>
-  <si>
-    <t>14:18:39.802</t>
-  </si>
-  <si>
-    <t>14:18:16.740</t>
-  </si>
-  <si>
-    <t>14:18:42.643</t>
-  </si>
-  <si>
-    <t>14:17:38.569</t>
-  </si>
-  <si>
-    <t>14:18:47.118</t>
-  </si>
-  <si>
-    <t>14:20:19.716</t>
-  </si>
-  <si>
-    <t>14:20:22.918</t>
-  </si>
-  <si>
-    <t>14:20:19.275</t>
-  </si>
-  <si>
-    <t>14:20:32.618</t>
-  </si>
-  <si>
-    <t>14:20:18.521</t>
-  </si>
-  <si>
-    <t>14:20:37.856</t>
-  </si>
-  <si>
-    <t>14:20:17.825</t>
-  </si>
-  <si>
-    <t>14:20:39.195</t>
-  </si>
-  <si>
-    <t>14:20:17.191</t>
-  </si>
-  <si>
-    <t>14:20:39.961</t>
-  </si>
-  <si>
-    <t>14:20:16.452</t>
-  </si>
-  <si>
-    <t>14:20:42.865</t>
-  </si>
-  <si>
-    <t>14:19:38.523</t>
-  </si>
-  <si>
-    <t>14:20:53.316</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El botón de pendings muestra existosamente que el 4FKU100 no tiene apuestas pendientes </t>
-  </si>
-  <si>
-    <t>14:37:11.447</t>
-  </si>
-  <si>
-    <t>14:37:35.019</t>
-  </si>
-  <si>
-    <t>14:37:10.813</t>
-  </si>
-  <si>
-    <t>14:37:44.857</t>
-  </si>
-  <si>
-    <t>14:37:09.795</t>
-  </si>
-  <si>
-    <t>14:38:00.536</t>
-  </si>
-  <si>
-    <t>14:37:08.851</t>
-  </si>
-  <si>
-    <t>14:38:02.156</t>
-  </si>
-  <si>
-    <t>14:37:07.888</t>
-  </si>
-  <si>
-    <t>14:38:03.042</t>
-  </si>
-  <si>
-    <t>14:37:06.914</t>
-  </si>
-  <si>
-    <t>14:38:06.018</t>
-  </si>
-  <si>
-    <t>14:35:54.952</t>
-  </si>
-  <si>
-    <t>14:38:26.831</t>
+    <t>13:18:33.788</t>
+  </si>
+  <si>
+    <t>13:19:01.995</t>
+  </si>
+  <si>
+    <t>13:18:32.802</t>
+  </si>
+  <si>
+    <t>13:19:08.082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los días de la semana Monday,Tuesday,Wednesday,Thursday,Friday,Saturday,Sunday y  encabezado de sumatorial Total se ven correctamente en la tabla de días de la semana </t>
+  </si>
+  <si>
+    <t>13:17:41.376</t>
+  </si>
+  <si>
+    <t>13:19:39.076</t>
+  </si>
+  <si>
+    <t>La prueba no se pudo realizar debido a un fallo anomalo en la prueba Favor de revisar en la consola de katalon con el siguiente código -99</t>
+  </si>
+  <si>
+    <t>13:22:30.936</t>
+  </si>
+  <si>
+    <t>13:22:39.972</t>
+  </si>
+  <si>
+    <t>13:22:30.176</t>
+  </si>
+  <si>
+    <t>13:22:52.074</t>
+  </si>
+  <si>
+    <t>13:22:29.079</t>
+  </si>
+  <si>
+    <t>13:22:59.771</t>
+  </si>
+  <si>
+    <t>13:22:28.018</t>
+  </si>
+  <si>
+    <t>13:23:01.631</t>
+  </si>
+  <si>
+    <t>13:22:27.071</t>
+  </si>
+  <si>
+    <t>13:23:07.713</t>
+  </si>
+  <si>
+    <t>13:20:36.161</t>
+  </si>
+  <si>
+    <t>13:23:29.325</t>
+  </si>
+  <si>
+    <t>13:27:19.302</t>
+  </si>
+  <si>
+    <t>13:28:21.278</t>
+  </si>
+  <si>
+    <t>13:37:38.801</t>
+  </si>
+  <si>
+    <t>13:37:41.824</t>
+  </si>
+  <si>
+    <t>13:37:38.361</t>
+  </si>
+  <si>
+    <t>13:37:53.869</t>
+  </si>
+  <si>
+    <t>13:37:37.647</t>
+  </si>
+  <si>
+    <t>13:38:01.121</t>
+  </si>
+  <si>
+    <t>13:37:36.995</t>
+  </si>
+  <si>
+    <t>13:38:02.592</t>
+  </si>
+  <si>
+    <t>13:37:36.270</t>
+  </si>
+  <si>
+    <t>13:38:07.214</t>
+  </si>
+  <si>
+    <t>13:37:04.462</t>
+  </si>
+  <si>
+    <t>13:38:08.044</t>
+  </si>
+  <si>
+    <t>13:40:11.473</t>
+  </si>
+  <si>
+    <t>13:40:14.845</t>
+  </si>
+  <si>
+    <t>13:40:10.963</t>
+  </si>
+  <si>
+    <t>13:40:27.647</t>
+  </si>
+  <si>
+    <t>13:40:10.235</t>
+  </si>
+  <si>
+    <t>13:40:35.268</t>
+  </si>
+  <si>
+    <t>13:40:09.567</t>
+  </si>
+  <si>
+    <t>13:40:36.975</t>
+  </si>
+  <si>
+    <t>13:40:08.985</t>
+  </si>
+  <si>
+    <t>13:40:41.450</t>
+  </si>
+  <si>
+    <t>13:39:38.387</t>
+  </si>
+  <si>
+    <t>13:40:42.252</t>
+  </si>
+  <si>
+    <t>13:44:48.142</t>
+  </si>
+  <si>
+    <t>13:44:53.092</t>
+  </si>
+  <si>
+    <t>13:44:47.705</t>
+  </si>
+  <si>
+    <t>13:45:05.825</t>
+  </si>
+  <si>
+    <t>13:44:46.975</t>
+  </si>
+  <si>
+    <t>13:45:13.690</t>
+  </si>
+  <si>
+    <t>13:44:46.303</t>
+  </si>
+  <si>
+    <t>13:45:15.123</t>
+  </si>
+  <si>
+    <t>13:44:45.675</t>
+  </si>
+  <si>
+    <t>13:45:19.513</t>
+  </si>
+  <si>
+    <t>13:44:12.906</t>
+  </si>
+  <si>
+    <t>13:45:20.339</t>
+  </si>
+  <si>
+    <t>13:51:40.446</t>
+  </si>
+  <si>
+    <t>13:51:45.330</t>
+  </si>
+  <si>
+    <t>13:51:39.688</t>
+  </si>
+  <si>
+    <t>13:51:59.583</t>
+  </si>
+  <si>
+    <t>13:51:38.577</t>
+  </si>
+  <si>
+    <t>13:52:07.133</t>
+  </si>
+  <si>
+    <t>13:51:37.533</t>
+  </si>
+  <si>
+    <t>13:52:08.812</t>
+  </si>
+  <si>
+    <t>13:51:36.633</t>
+  </si>
+  <si>
+    <t>13:52:15.056</t>
+  </si>
+  <si>
+    <t>13:48:56.019</t>
+  </si>
+  <si>
+    <t>13:52:32.851</t>
+  </si>
+  <si>
+    <t>14:19:02.168</t>
+  </si>
+  <si>
+    <t>14:19:06.197</t>
+  </si>
+  <si>
+    <t>14:19:01.521</t>
+  </si>
+  <si>
+    <t>14:19:18.473</t>
+  </si>
+  <si>
+    <t>14:19:00.471</t>
+  </si>
+  <si>
+    <t>14:19:25.780</t>
+  </si>
+  <si>
+    <t>14:18:59.467</t>
+  </si>
+  <si>
+    <t>14:19:27.440</t>
+  </si>
+  <si>
+    <t>14:18:58.591</t>
+  </si>
+  <si>
+    <t>14:19:33.283</t>
+  </si>
+  <si>
+    <t>14:18:26.887</t>
+  </si>
+  <si>
+    <t>14:19:55.559</t>
+  </si>
+  <si>
+    <t>15:02:09.476</t>
+  </si>
+  <si>
+    <t>15:02:12.511</t>
+  </si>
+  <si>
+    <t>15:02:08.762</t>
+  </si>
+  <si>
+    <t>15:02:25.495</t>
+  </si>
+  <si>
+    <t>15:02:07.583</t>
+  </si>
+  <si>
+    <t>15:02:32.845</t>
+  </si>
+  <si>
+    <t>15:02:06.427</t>
+  </si>
+  <si>
+    <t>15:02:34.698</t>
+  </si>
+  <si>
+    <t>15:02:05.485</t>
+  </si>
+  <si>
+    <t>15:02:41.066</t>
+  </si>
+  <si>
+    <t>09/11/2019</t>
+  </si>
+  <si>
+    <t>10:22:58.812</t>
+  </si>
+  <si>
+    <t>10:23:02.407</t>
+  </si>
+  <si>
+    <t>Firefox 70.0.1</t>
+  </si>
+  <si>
+    <t>10:22:57.272</t>
+  </si>
+  <si>
+    <t>10:23:15.521</t>
+  </si>
+  <si>
+    <t>10:22:58.407</t>
+  </si>
+  <si>
+    <t>10:23:16.731</t>
+  </si>
+  <si>
+    <t>10:22:56.481</t>
+  </si>
+  <si>
+    <t>10:23:23.153</t>
+  </si>
+  <si>
+    <t>10:22:57.728</t>
+  </si>
+  <si>
+    <t>10:23:24.715</t>
+  </si>
+  <si>
+    <t>10:22:55.760</t>
+  </si>
+  <si>
+    <t>10:23:27.076</t>
+  </si>
+  <si>
+    <t>10:22:56.999</t>
+  </si>
+  <si>
+    <t>10:23:27.369</t>
+  </si>
+  <si>
+    <t>10:22:55.172</t>
+  </si>
+  <si>
+    <t>10:23:31.783</t>
+  </si>
+  <si>
+    <t>10:22:56.406</t>
+  </si>
+  <si>
+    <t>10:23:32.194</t>
+  </si>
+  <si>
+    <t>10:22:19.315</t>
+  </si>
+  <si>
+    <t>10:23:33.180</t>
+  </si>
+  <si>
+    <t>10:22:20.104</t>
+  </si>
+  <si>
+    <t>10:23:33.537</t>
+  </si>
+  <si>
+    <t>11:26:58.724</t>
+  </si>
+  <si>
+    <t>11:27:01.803</t>
+  </si>
+  <si>
+    <t>11:26:58.284</t>
+  </si>
+  <si>
+    <t>11:27:14.137</t>
+  </si>
+  <si>
+    <t>11:26:57.549</t>
+  </si>
+  <si>
+    <t>11:27:21.438</t>
+  </si>
+  <si>
+    <t>11:26:56.900</t>
+  </si>
+  <si>
+    <t>11:27:23.230</t>
+  </si>
+  <si>
+    <t>11:26:56.282</t>
+  </si>
+  <si>
+    <t>11:27:27.757</t>
+  </si>
+  <si>
+    <t>11:26:24.423</t>
+  </si>
+  <si>
+    <t>11:27:29.603</t>
+  </si>
+  <si>
+    <t>12:33:12.043</t>
+  </si>
+  <si>
+    <t>12:33:15.280</t>
+  </si>
+  <si>
+    <t>12:33:11.611</t>
+  </si>
+  <si>
+    <t>12:33:28.293</t>
+  </si>
+  <si>
+    <t>12:33:10.935</t>
+  </si>
+  <si>
+    <t>12:33:35.894</t>
+  </si>
+  <si>
+    <t>12:33:10.231</t>
+  </si>
+  <si>
+    <t>12:33:37.495</t>
+  </si>
+  <si>
+    <t>12:33:09.661</t>
+  </si>
+  <si>
+    <t>12:33:41.764</t>
+  </si>
+  <si>
+    <t>12:37:02.811</t>
+  </si>
+  <si>
+    <t>12:37:05.919</t>
+  </si>
+  <si>
+    <t>12:37:02.405</t>
+  </si>
+  <si>
+    <t>12:37:17.721</t>
+  </si>
+  <si>
+    <t>12:37:01.685</t>
+  </si>
+  <si>
+    <t>12:37:24.605</t>
+  </si>
+  <si>
+    <t>12:37:01.017</t>
+  </si>
+  <si>
+    <t>12:37:26.025</t>
+  </si>
+  <si>
+    <t>12:37:00.416</t>
+  </si>
+  <si>
+    <t>12:37:30.651</t>
+  </si>
+  <si>
+    <t>12:36:25.569</t>
+  </si>
+  <si>
+    <t>12:38:09.949</t>
+  </si>
+  <si>
+    <t>El sistema no pudo validar las trancciones del día lunes debido a que algún paso previo o precondición no se cumplio Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>12:43:58.800</t>
+  </si>
+  <si>
+    <t>12:44:27.800</t>
+  </si>
+  <si>
+    <t>12:43:53.564</t>
+  </si>
+  <si>
+    <t>12:44:40.018</t>
+  </si>
+  <si>
+    <t>12:43:45.058</t>
+  </si>
+  <si>
+    <t>12:45:00.089</t>
+  </si>
+  <si>
+    <t>12:43:37.446</t>
+  </si>
+  <si>
+    <t>12:45:01.997</t>
+  </si>
+  <si>
+    <t>12:43:30.746</t>
+  </si>
+  <si>
+    <t>12:45:07.934</t>
+  </si>
+  <si>
+    <t>11/11/2019</t>
+  </si>
+  <si>
+    <t>07:12:38.650</t>
+  </si>
+  <si>
+    <t>07:12:42.306</t>
+  </si>
+  <si>
+    <t>07:12:38.235</t>
+  </si>
+  <si>
+    <t>07:12:53.195</t>
+  </si>
+  <si>
+    <t>07:12:37.566</t>
+  </si>
+  <si>
+    <t>07:13:00.538</t>
+  </si>
+  <si>
+    <t>07:12:36.846</t>
+  </si>
+  <si>
+    <t>07:13:01.893</t>
+  </si>
+  <si>
+    <t>07:12:36.301</t>
+  </si>
+  <si>
+    <t>07:13:06.218</t>
+  </si>
+  <si>
+    <t>09:53:31.401</t>
+  </si>
+  <si>
+    <t>09:53:34.478</t>
+  </si>
+  <si>
+    <t>09:53:30.901</t>
+  </si>
+  <si>
+    <t>09:53:45.167</t>
+  </si>
+  <si>
+    <t>09:53:30.165</t>
+  </si>
+  <si>
+    <t>09:53:52.830</t>
+  </si>
+  <si>
+    <t>09:53:29.433</t>
+  </si>
+  <si>
+    <t>09:53:54.318</t>
+  </si>
+  <si>
+    <t>09:53:28.829</t>
+  </si>
+  <si>
+    <t>09:53:58.444</t>
+  </si>
+  <si>
+    <t>09:52:54.371</t>
+  </si>
+  <si>
+    <t>09:54:00.213</t>
+  </si>
+  <si>
+    <t>10:23:16.288</t>
+  </si>
+  <si>
+    <t>10:23:19.223</t>
+  </si>
+  <si>
+    <t>10:23:15.825</t>
+  </si>
+  <si>
+    <t>10:23:30.067</t>
+  </si>
+  <si>
+    <t>10:23:15.103</t>
+  </si>
+  <si>
+    <t>10:23:37.106</t>
+  </si>
+  <si>
+    <t>10:23:14.482</t>
+  </si>
+  <si>
+    <t>10:23:38.651</t>
+  </si>
+  <si>
+    <t>10:23:13.761</t>
+  </si>
+  <si>
+    <t>10:23:43.166</t>
+  </si>
+  <si>
+    <t>10:22:40.805</t>
+  </si>
+  <si>
+    <t>10:23:44.920</t>
+  </si>
+  <si>
+    <t>10:30:05.778</t>
+  </si>
+  <si>
+    <t>10:30:26.131</t>
+  </si>
+  <si>
+    <t>10:30:01.184</t>
+  </si>
+  <si>
+    <t>10:30:38.147</t>
+  </si>
+  <si>
+    <t>10:29:53.656</t>
+  </si>
+  <si>
+    <t>10:31:08.824</t>
+  </si>
+  <si>
+    <t>10:29:47.156</t>
+  </si>
+  <si>
+    <t>10:31:10.600</t>
+  </si>
+  <si>
+    <t>10:29:41.120</t>
+  </si>
+  <si>
+    <t>10:31:17.010</t>
+  </si>
+  <si>
+    <t>10:39:41.852</t>
+  </si>
+  <si>
+    <t>10:39:44.901</t>
+  </si>
+  <si>
+    <t>10:39:41.354</t>
+  </si>
+  <si>
+    <t>10:39:55.351</t>
+  </si>
+  <si>
+    <t>10:39:40.638</t>
+  </si>
+  <si>
+    <t>10:40:02.829</t>
+  </si>
+  <si>
+    <t>10:39:39.912</t>
+  </si>
+  <si>
+    <t>10:40:04.202</t>
+  </si>
+  <si>
+    <t>10:39:39.227</t>
+  </si>
+  <si>
+    <t>10:40:08.668</t>
+  </si>
+  <si>
+    <t>10:39:05.796</t>
+  </si>
+  <si>
+    <t>10:40:10.323</t>
+  </si>
+  <si>
+    <t>10:46:11.108</t>
+  </si>
+  <si>
+    <t>10:46:16.555</t>
+  </si>
+  <si>
+    <t>10:46:06.636</t>
+  </si>
+  <si>
+    <t>10:46:53.240</t>
+  </si>
+  <si>
+    <t>10:45:59.841</t>
+  </si>
+  <si>
+    <t>10:47:09.305</t>
+  </si>
+  <si>
+    <t>10:45:53.572</t>
+  </si>
+  <si>
+    <t>10:47:19.661</t>
+  </si>
+  <si>
+    <t>10:45:48.288</t>
+  </si>
+  <si>
+    <t>10:48:04.411</t>
+  </si>
+  <si>
+    <t>10:44:59.303</t>
+  </si>
+  <si>
+    <t>10:50:15.965</t>
+  </si>
+  <si>
+    <t>10:52:56.734</t>
+  </si>
+  <si>
+    <t>10:52:59.766</t>
+  </si>
+  <si>
+    <t>10:52:56.212</t>
+  </si>
+  <si>
+    <t>10:53:10.972</t>
+  </si>
+  <si>
+    <t>10:52:55.483</t>
+  </si>
+  <si>
+    <t>10:53:18.360</t>
+  </si>
+  <si>
+    <t>10:52:54.800</t>
+  </si>
+  <si>
+    <t>10:53:19.669</t>
+  </si>
+  <si>
+    <t>10:52:54.256</t>
+  </si>
+  <si>
+    <t>10:53:23.905</t>
+  </si>
+  <si>
+    <t>10:52:21.994</t>
+  </si>
+  <si>
+    <t>10:54:02.066</t>
+  </si>
+  <si>
+    <t>El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algón procedimiento previ como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>14:24:00.554</t>
+  </si>
+  <si>
+    <t>14:24:03.138</t>
+  </si>
+  <si>
+    <t>14:24:00.126</t>
+  </si>
+  <si>
+    <t>14:24:13.753</t>
+  </si>
+  <si>
+    <t>14:23:59.366</t>
+  </si>
+  <si>
+    <t>14:24:21.155</t>
+  </si>
+  <si>
+    <t>14:23:58.725</t>
+  </si>
+  <si>
+    <t>14:24:22.503</t>
+  </si>
+  <si>
+    <t>14:23:58.117</t>
+  </si>
+  <si>
+    <t>14:24:26.554</t>
+  </si>
+  <si>
+    <t>14:23:26.432</t>
+  </si>
+  <si>
+    <t>14:24:28.874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes aparecen exitosamente </t>
+  </si>
+  <si>
+    <t>14:34:17.198</t>
+  </si>
+  <si>
+    <t>14:34:29.609</t>
+  </si>
+  <si>
+    <t>14:34:16.771</t>
+  </si>
+  <si>
+    <t>14:34:40.455</t>
+  </si>
+  <si>
+    <t>14:34:16.025</t>
+  </si>
+  <si>
+    <t>14:34:47.988</t>
+  </si>
+  <si>
+    <t>14:34:15.293</t>
+  </si>
+  <si>
+    <t>14:34:49.360</t>
+  </si>
+  <si>
+    <t>14:34:14.745</t>
+  </si>
+  <si>
+    <t>14:34:53.926</t>
+  </si>
+  <si>
+    <t>14:34:13.666</t>
+  </si>
+  <si>
+    <t>14:34:58.559</t>
   </si>
 </sst>
 </file>
@@ -1027,28 +1681,28 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>295</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>392</v>
       </c>
       <c r="F2" t="s">
-        <v>176</v>
+        <v>393</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1113,22 +1767,22 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1143,7 +1797,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1181,7 +1835,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1201,19 +1855,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1228,7 +1882,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1931,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1294,22 +1948,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>181</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>182</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1324,7 +1978,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1369,7 +2023,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1386,22 +2040,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>183</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>184</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1416,7 +2070,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1463,7 +2117,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1480,28 +2134,28 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>295</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>394</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>395</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1510,7 +2164,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1569,22 +2223,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>295</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>390</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>391</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -1593,7 +2247,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1646,13 +2300,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1711,7 +2365,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1728,22 +2382,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1758,7 +2412,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>135</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1781,7 +2435,7 @@
         <v>6</v>
       </c>
       <c r="G43" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H43" t="s">
         <v>8</v>
@@ -1803,10 +2457,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3043AB7-CB0A-4C57-8B73-07EA10FF0C55}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,7 +2485,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1846,24 +2500,109 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9C5BB7-4BB0-42AE-9B9A-9D6F51B71656}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>186</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1878,7 +2617,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>172</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1948,19 +2687,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1975,7 +2714,698 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D77E9EE9-4A49-4EE9-9D8B-471D2F12F474}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483AA6C1-D8F1-407A-B52A-A4D73BED75EF}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" t="s">
+        <v>396</v>
+      </c>
+      <c r="F2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9B29C7-5A72-4DBC-8A01-21E29E06A8F5}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB834EB-1135-4739-B054-0860D368C29E}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" t="s">
+        <v>398</v>
+      </c>
+      <c r="F2" t="s">
+        <v>399</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59417A3-7321-4498-9F5A-BBC02D169926}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="10" customWidth="true" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBC83E2-23E7-45A8-B890-DF53F9A6E97F}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" t="s">
+        <v>400</v>
+      </c>
+      <c r="F2" t="s">
+        <v>401</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6562A8C0-FC7B-445D-A338-0FDEAA881DD7}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2" t="s">
+        <v>388</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B06236E-AD84-403E-A6C7-523AD42AD6C3}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2049,16 +3479,16 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2070,10 +3500,10 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
@@ -2137,22 +3567,22 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
         <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2164,10 +3594,10 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2230,19 +3660,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2257,7 +3687,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2319,19 +3749,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2346,7 +3776,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2404,19 +3834,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2431,7 +3861,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2494,16 +3924,16 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2518,7 +3948,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2567,16 +3997,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -2591,7 +4021,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
C6401 ,C6402 y C6405 Test cases automatizados el 11/14/2019 C6406, Test cases automatizados 11/115/2019 C6403
Signed-off-by: qa-katalon <qa-katalon@DEV-QA-KatalonStudio.BMinc.eu>
</commit_message>
<xml_diff>
--- a/Data Files/TestData/Reports/TestResults.xlsx
+++ b/Data Files/TestData/Reports/TestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\QAPregameNuevo\Data Files\TestData\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8083ECBB-9042-4716-84FF-BFC282DF6148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B46410F-0848-45A5-81D2-F3E88B712E80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1845" windowWidth="21600" windowHeight="11385" firstSheet="15" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="3060" windowWidth="21600" windowHeight="11385" firstSheet="21" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C6414" sheetId="1" r:id="rId1"/>
@@ -40,13 +40,18 @@
     <sheet name="C6399" sheetId="26" r:id="rId25"/>
     <sheet name="C6400" sheetId="27" r:id="rId26"/>
     <sheet name="C3875" sheetId="21" r:id="rId27"/>
+    <sheet name="C6401" sheetId="28" r:id="rId28"/>
+    <sheet name="C6405" sheetId="29" r:id="rId29"/>
+    <sheet name="C6402" sheetId="30" r:id="rId30"/>
+    <sheet name="C6408" sheetId="31" r:id="rId31"/>
+    <sheet name="C6403" sheetId="32" r:id="rId32"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="157">
   <si>
     <t>URL</t>
   </si>
@@ -354,904 +359,169 @@
     <t>13:29:12.316</t>
   </si>
   <si>
-    <t>08/11/2019</t>
-  </si>
-  <si>
-    <t>12:28:27.066</t>
-  </si>
-  <si>
-    <t>12:29:03.954</t>
-  </si>
-  <si>
-    <t>Chrome 78.0.3904.87</t>
-  </si>
-  <si>
-    <t>12:28:26.341</t>
-  </si>
-  <si>
-    <t>12:29:18.644</t>
-  </si>
-  <si>
-    <t>12:28:25.352</t>
-  </si>
-  <si>
-    <t>12:29:41.876</t>
-  </si>
-  <si>
     <t>Permiso de Sportbook Deportes es correctamente accesible para el usuario</t>
   </si>
   <si>
-    <t>12:28:24.262</t>
-  </si>
-  <si>
-    <t>12:29:43.705</t>
-  </si>
-  <si>
-    <t>12:28:23.254</t>
-  </si>
-  <si>
-    <t>12:29:49.844</t>
-  </si>
-  <si>
     <t xml:space="preserve">Los días de la semana Lunes,Martes,Miércoles,Jueves,Viernes,Sábado,Domingo y  encabezado de sumatorial Total se ven correctamente en la tabla de días de la semana </t>
   </si>
   <si>
-    <t>12:28:21.855</t>
-  </si>
-  <si>
-    <t>12:30:09.189</t>
-  </si>
-  <si>
     <t>El checkbox "Iniciar Martes" muestra correctamente los días de la semana con el siguiente orden: Martes,Miércoles,Jueves,Viernes,Sábado,Domingo,Lunes,Total</t>
   </si>
   <si>
-    <t>12:33:40.972</t>
-  </si>
-  <si>
-    <t>El jugador SHA2001 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes</t>
-  </si>
-  <si>
     <t>PRAC06</t>
   </si>
   <si>
     <t>TEST</t>
   </si>
   <si>
-    <t>12:36:33.823</t>
-  </si>
-  <si>
-    <t>El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes</t>
-  </si>
-  <si>
-    <t>12:38:18.484</t>
-  </si>
-  <si>
-    <t>12:46:10.742</t>
-  </si>
-  <si>
-    <t>13:18:36.791</t>
-  </si>
-  <si>
-    <t>13:18:39.738</t>
-  </si>
-  <si>
-    <t>13:18:36.120</t>
-  </si>
-  <si>
-    <t>13:18:52.047</t>
-  </si>
-  <si>
-    <t>13:18:34.964</t>
-  </si>
-  <si>
-    <t>13:18:59.900</t>
-  </si>
-  <si>
-    <t>Permiso de Sportbook Sports es correctamente accesible para el usuario</t>
-  </si>
-  <si>
-    <t>13:18:33.788</t>
-  </si>
-  <si>
-    <t>13:19:01.995</t>
-  </si>
-  <si>
-    <t>13:18:32.802</t>
-  </si>
-  <si>
-    <t>13:19:08.082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los días de la semana Monday,Tuesday,Wednesday,Thursday,Friday,Saturday,Sunday y  encabezado de sumatorial Total se ven correctamente en la tabla de días de la semana </t>
-  </si>
-  <si>
-    <t>13:17:41.376</t>
-  </si>
-  <si>
-    <t>13:19:39.076</t>
-  </si>
-  <si>
-    <t>La prueba no se pudo realizar debido a un fallo anomalo en la prueba Favor de revisar en la consola de katalon con el siguiente código -99</t>
-  </si>
-  <si>
-    <t>13:22:30.936</t>
-  </si>
-  <si>
-    <t>13:22:39.972</t>
-  </si>
-  <si>
-    <t>13:22:30.176</t>
-  </si>
-  <si>
-    <t>13:22:52.074</t>
-  </si>
-  <si>
-    <t>13:22:29.079</t>
-  </si>
-  <si>
-    <t>13:22:59.771</t>
-  </si>
-  <si>
-    <t>13:22:28.018</t>
-  </si>
-  <si>
-    <t>13:23:01.631</t>
-  </si>
-  <si>
-    <t>13:22:27.071</t>
-  </si>
-  <si>
-    <t>13:23:07.713</t>
-  </si>
-  <si>
-    <t>13:20:36.161</t>
-  </si>
-  <si>
-    <t>13:23:29.325</t>
-  </si>
-  <si>
-    <t>13:27:19.302</t>
-  </si>
-  <si>
-    <t>13:28:21.278</t>
-  </si>
-  <si>
-    <t>13:37:38.801</t>
-  </si>
-  <si>
-    <t>13:37:41.824</t>
-  </si>
-  <si>
-    <t>13:37:38.361</t>
-  </si>
-  <si>
-    <t>13:37:53.869</t>
-  </si>
-  <si>
-    <t>13:37:37.647</t>
-  </si>
-  <si>
-    <t>13:38:01.121</t>
-  </si>
-  <si>
-    <t>13:37:36.995</t>
-  </si>
-  <si>
-    <t>13:38:02.592</t>
-  </si>
-  <si>
-    <t>13:37:36.270</t>
-  </si>
-  <si>
-    <t>13:38:07.214</t>
-  </si>
-  <si>
-    <t>13:37:04.462</t>
-  </si>
-  <si>
-    <t>13:38:08.044</t>
-  </si>
-  <si>
-    <t>13:40:11.473</t>
-  </si>
-  <si>
-    <t>13:40:14.845</t>
-  </si>
-  <si>
-    <t>13:40:10.963</t>
-  </si>
-  <si>
-    <t>13:40:27.647</t>
-  </si>
-  <si>
-    <t>13:40:10.235</t>
-  </si>
-  <si>
-    <t>13:40:35.268</t>
-  </si>
-  <si>
-    <t>13:40:09.567</t>
-  </si>
-  <si>
-    <t>13:40:36.975</t>
-  </si>
-  <si>
-    <t>13:40:08.985</t>
-  </si>
-  <si>
-    <t>13:40:41.450</t>
-  </si>
-  <si>
-    <t>13:39:38.387</t>
-  </si>
-  <si>
-    <t>13:40:42.252</t>
-  </si>
-  <si>
-    <t>13:44:48.142</t>
-  </si>
-  <si>
-    <t>13:44:53.092</t>
-  </si>
-  <si>
-    <t>13:44:47.705</t>
-  </si>
-  <si>
-    <t>13:45:05.825</t>
-  </si>
-  <si>
-    <t>13:44:46.975</t>
-  </si>
-  <si>
-    <t>13:45:13.690</t>
-  </si>
-  <si>
-    <t>13:44:46.303</t>
-  </si>
-  <si>
-    <t>13:45:15.123</t>
-  </si>
-  <si>
-    <t>13:44:45.675</t>
-  </si>
-  <si>
-    <t>13:45:19.513</t>
-  </si>
-  <si>
-    <t>13:44:12.906</t>
-  </si>
-  <si>
-    <t>13:45:20.339</t>
-  </si>
-  <si>
-    <t>13:51:40.446</t>
-  </si>
-  <si>
-    <t>13:51:45.330</t>
-  </si>
-  <si>
-    <t>13:51:39.688</t>
-  </si>
-  <si>
-    <t>13:51:59.583</t>
-  </si>
-  <si>
-    <t>13:51:38.577</t>
-  </si>
-  <si>
-    <t>13:52:07.133</t>
-  </si>
-  <si>
-    <t>13:51:37.533</t>
-  </si>
-  <si>
-    <t>13:52:08.812</t>
-  </si>
-  <si>
-    <t>13:51:36.633</t>
-  </si>
-  <si>
-    <t>13:52:15.056</t>
-  </si>
-  <si>
-    <t>13:48:56.019</t>
-  </si>
-  <si>
-    <t>13:52:32.851</t>
-  </si>
-  <si>
-    <t>14:19:02.168</t>
-  </si>
-  <si>
-    <t>14:19:06.197</t>
-  </si>
-  <si>
-    <t>14:19:01.521</t>
-  </si>
-  <si>
-    <t>14:19:18.473</t>
-  </si>
-  <si>
-    <t>14:19:00.471</t>
-  </si>
-  <si>
-    <t>14:19:25.780</t>
-  </si>
-  <si>
-    <t>14:18:59.467</t>
-  </si>
-  <si>
-    <t>14:19:27.440</t>
-  </si>
-  <si>
-    <t>14:18:58.591</t>
-  </si>
-  <si>
-    <t>14:19:33.283</t>
-  </si>
-  <si>
-    <t>14:18:26.887</t>
-  </si>
-  <si>
-    <t>14:19:55.559</t>
-  </si>
-  <si>
-    <t>15:02:09.476</t>
-  </si>
-  <si>
-    <t>15:02:12.511</t>
-  </si>
-  <si>
-    <t>15:02:08.762</t>
-  </si>
-  <si>
-    <t>15:02:25.495</t>
-  </si>
-  <si>
-    <t>15:02:07.583</t>
-  </si>
-  <si>
-    <t>15:02:32.845</t>
-  </si>
-  <si>
-    <t>15:02:06.427</t>
-  </si>
-  <si>
-    <t>15:02:34.698</t>
-  </si>
-  <si>
-    <t>15:02:05.485</t>
-  </si>
-  <si>
-    <t>15:02:41.066</t>
-  </si>
-  <si>
-    <t>09/11/2019</t>
-  </si>
-  <si>
-    <t>10:22:58.812</t>
-  </si>
-  <si>
-    <t>10:23:02.407</t>
-  </si>
-  <si>
     <t>Firefox 70.0.1</t>
   </si>
   <si>
-    <t>10:22:57.272</t>
-  </si>
-  <si>
-    <t>10:23:15.521</t>
-  </si>
-  <si>
-    <t>10:22:58.407</t>
-  </si>
-  <si>
-    <t>10:23:16.731</t>
-  </si>
-  <si>
-    <t>10:22:56.481</t>
-  </si>
-  <si>
-    <t>10:23:23.153</t>
-  </si>
-  <si>
-    <t>10:22:57.728</t>
-  </si>
-  <si>
-    <t>10:23:24.715</t>
-  </si>
-  <si>
-    <t>10:22:55.760</t>
-  </si>
-  <si>
-    <t>10:23:27.076</t>
-  </si>
-  <si>
-    <t>10:22:56.999</t>
-  </si>
-  <si>
-    <t>10:23:27.369</t>
-  </si>
-  <si>
-    <t>10:22:55.172</t>
-  </si>
-  <si>
-    <t>10:23:31.783</t>
-  </si>
-  <si>
-    <t>10:22:56.406</t>
-  </si>
-  <si>
-    <t>10:23:32.194</t>
-  </si>
-  <si>
-    <t>10:22:19.315</t>
-  </si>
-  <si>
-    <t>10:23:33.180</t>
-  </si>
-  <si>
-    <t>10:22:20.104</t>
-  </si>
-  <si>
-    <t>10:23:33.537</t>
-  </si>
-  <si>
-    <t>11:26:58.724</t>
-  </si>
-  <si>
-    <t>11:27:01.803</t>
-  </si>
-  <si>
-    <t>11:26:58.284</t>
-  </si>
-  <si>
-    <t>11:27:14.137</t>
-  </si>
-  <si>
-    <t>11:26:57.549</t>
-  </si>
-  <si>
-    <t>11:27:21.438</t>
-  </si>
-  <si>
-    <t>11:26:56.900</t>
-  </si>
-  <si>
-    <t>11:27:23.230</t>
-  </si>
-  <si>
-    <t>11:26:56.282</t>
-  </si>
-  <si>
-    <t>11:27:27.757</t>
-  </si>
-  <si>
-    <t>11:26:24.423</t>
-  </si>
-  <si>
-    <t>11:27:29.603</t>
-  </si>
-  <si>
-    <t>12:33:12.043</t>
-  </si>
-  <si>
-    <t>12:33:15.280</t>
-  </si>
-  <si>
-    <t>12:33:11.611</t>
-  </si>
-  <si>
-    <t>12:33:28.293</t>
-  </si>
-  <si>
-    <t>12:33:10.935</t>
-  </si>
-  <si>
-    <t>12:33:35.894</t>
-  </si>
-  <si>
-    <t>12:33:10.231</t>
-  </si>
-  <si>
-    <t>12:33:37.495</t>
-  </si>
-  <si>
-    <t>12:33:09.661</t>
-  </si>
-  <si>
-    <t>12:33:41.764</t>
-  </si>
-  <si>
-    <t>12:37:02.811</t>
-  </si>
-  <si>
-    <t>12:37:05.919</t>
-  </si>
-  <si>
-    <t>12:37:02.405</t>
-  </si>
-  <si>
-    <t>12:37:17.721</t>
-  </si>
-  <si>
-    <t>12:37:01.685</t>
-  </si>
-  <si>
-    <t>12:37:24.605</t>
-  </si>
-  <si>
-    <t>12:37:01.017</t>
-  </si>
-  <si>
-    <t>12:37:26.025</t>
-  </si>
-  <si>
-    <t>12:37:00.416</t>
-  </si>
-  <si>
-    <t>12:37:30.651</t>
-  </si>
-  <si>
-    <t>12:36:25.569</t>
-  </si>
-  <si>
-    <t>12:38:09.949</t>
-  </si>
-  <si>
-    <t>El sistema no pudo validar las trancciones del día lunes debido a que algún paso previo o precondición no se cumplio Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
-  </si>
-  <si>
-    <t>12:43:58.800</t>
-  </si>
-  <si>
-    <t>12:44:27.800</t>
-  </si>
-  <si>
-    <t>12:43:53.564</t>
-  </si>
-  <si>
-    <t>12:44:40.018</t>
-  </si>
-  <si>
-    <t>12:43:45.058</t>
-  </si>
-  <si>
-    <t>12:45:00.089</t>
-  </si>
-  <si>
-    <t>12:43:37.446</t>
-  </si>
-  <si>
-    <t>12:45:01.997</t>
-  </si>
-  <si>
-    <t>12:43:30.746</t>
-  </si>
-  <si>
-    <t>12:45:07.934</t>
-  </si>
-  <si>
     <t>11/11/2019</t>
   </si>
   <si>
-    <t>07:12:38.650</t>
-  </si>
-  <si>
-    <t>07:12:42.306</t>
-  </si>
-  <si>
-    <t>07:12:38.235</t>
-  </si>
-  <si>
-    <t>07:12:53.195</t>
-  </si>
-  <si>
-    <t>07:12:37.566</t>
-  </si>
-  <si>
-    <t>07:13:00.538</t>
-  </si>
-  <si>
-    <t>07:12:36.846</t>
-  </si>
-  <si>
-    <t>07:13:01.893</t>
-  </si>
-  <si>
-    <t>07:12:36.301</t>
-  </si>
-  <si>
-    <t>07:13:06.218</t>
-  </si>
-  <si>
-    <t>09:53:31.401</t>
-  </si>
-  <si>
-    <t>09:53:34.478</t>
-  </si>
-  <si>
-    <t>09:53:30.901</t>
-  </si>
-  <si>
-    <t>09:53:45.167</t>
-  </si>
-  <si>
-    <t>09:53:30.165</t>
-  </si>
-  <si>
-    <t>09:53:52.830</t>
-  </si>
-  <si>
-    <t>09:53:29.433</t>
-  </si>
-  <si>
-    <t>09:53:54.318</t>
-  </si>
-  <si>
-    <t>09:53:28.829</t>
-  </si>
-  <si>
-    <t>09:53:58.444</t>
-  </si>
-  <si>
-    <t>09:52:54.371</t>
-  </si>
-  <si>
-    <t>09:54:00.213</t>
-  </si>
-  <si>
-    <t>10:23:16.288</t>
-  </si>
-  <si>
-    <t>10:23:19.223</t>
-  </si>
-  <si>
-    <t>10:23:15.825</t>
-  </si>
-  <si>
-    <t>10:23:30.067</t>
-  </si>
-  <si>
-    <t>10:23:15.103</t>
-  </si>
-  <si>
-    <t>10:23:37.106</t>
-  </si>
-  <si>
-    <t>10:23:14.482</t>
-  </si>
-  <si>
-    <t>10:23:38.651</t>
-  </si>
-  <si>
-    <t>10:23:13.761</t>
-  </si>
-  <si>
-    <t>10:23:43.166</t>
-  </si>
-  <si>
-    <t>10:22:40.805</t>
-  </si>
-  <si>
-    <t>10:23:44.920</t>
-  </si>
-  <si>
-    <t>10:30:05.778</t>
-  </si>
-  <si>
-    <t>10:30:26.131</t>
-  </si>
-  <si>
-    <t>10:30:01.184</t>
-  </si>
-  <si>
-    <t>10:30:38.147</t>
-  </si>
-  <si>
-    <t>10:29:53.656</t>
-  </si>
-  <si>
-    <t>10:31:08.824</t>
-  </si>
-  <si>
-    <t>10:29:47.156</t>
-  </si>
-  <si>
-    <t>10:31:10.600</t>
-  </si>
-  <si>
-    <t>10:29:41.120</t>
-  </si>
-  <si>
-    <t>10:31:17.010</t>
-  </si>
-  <si>
-    <t>10:39:41.852</t>
-  </si>
-  <si>
-    <t>10:39:44.901</t>
-  </si>
-  <si>
-    <t>10:39:41.354</t>
-  </si>
-  <si>
-    <t>10:39:55.351</t>
-  </si>
-  <si>
-    <t>10:39:40.638</t>
-  </si>
-  <si>
-    <t>10:40:02.829</t>
-  </si>
-  <si>
-    <t>10:39:39.912</t>
-  </si>
-  <si>
-    <t>10:40:04.202</t>
-  </si>
-  <si>
-    <t>10:39:39.227</t>
-  </si>
-  <si>
-    <t>10:40:08.668</t>
-  </si>
-  <si>
-    <t>10:39:05.796</t>
-  </si>
-  <si>
-    <t>10:40:10.323</t>
-  </si>
-  <si>
-    <t>10:46:11.108</t>
-  </si>
-  <si>
-    <t>10:46:16.555</t>
-  </si>
-  <si>
-    <t>10:46:06.636</t>
-  </si>
-  <si>
-    <t>10:46:53.240</t>
-  </si>
-  <si>
-    <t>10:45:59.841</t>
-  </si>
-  <si>
-    <t>10:47:09.305</t>
-  </si>
-  <si>
-    <t>10:45:53.572</t>
-  </si>
-  <si>
-    <t>10:47:19.661</t>
-  </si>
-  <si>
-    <t>10:45:48.288</t>
-  </si>
-  <si>
-    <t>10:48:04.411</t>
-  </si>
-  <si>
-    <t>10:44:59.303</t>
-  </si>
-  <si>
-    <t>10:50:15.965</t>
-  </si>
-  <si>
-    <t>10:52:56.734</t>
-  </si>
-  <si>
-    <t>10:52:59.766</t>
-  </si>
-  <si>
-    <t>10:52:56.212</t>
-  </si>
-  <si>
-    <t>10:53:10.972</t>
-  </si>
-  <si>
-    <t>10:52:55.483</t>
-  </si>
-  <si>
-    <t>10:53:18.360</t>
-  </si>
-  <si>
-    <t>10:52:54.800</t>
-  </si>
-  <si>
-    <t>10:53:19.669</t>
-  </si>
-  <si>
-    <t>10:52:54.256</t>
-  </si>
-  <si>
-    <t>10:53:23.905</t>
-  </si>
-  <si>
-    <t>10:52:21.994</t>
-  </si>
-  <si>
-    <t>10:54:02.066</t>
-  </si>
-  <si>
-    <t>El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algón procedimiento previ como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
-  </si>
-  <si>
-    <t>14:24:00.554</t>
-  </si>
-  <si>
-    <t>14:24:03.138</t>
-  </si>
-  <si>
-    <t>14:24:00.126</t>
-  </si>
-  <si>
-    <t>14:24:13.753</t>
-  </si>
-  <si>
-    <t>14:23:59.366</t>
-  </si>
-  <si>
-    <t>14:24:21.155</t>
-  </si>
-  <si>
-    <t>14:23:58.725</t>
-  </si>
-  <si>
-    <t>14:24:22.503</t>
-  </si>
-  <si>
-    <t>14:23:58.117</t>
-  </si>
-  <si>
-    <t>14:24:26.554</t>
-  </si>
-  <si>
-    <t>14:23:26.432</t>
-  </si>
-  <si>
-    <t>14:24:28.874</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes aparecen exitosamente </t>
-  </si>
-  <si>
-    <t>14:34:17.198</t>
-  </si>
-  <si>
-    <t>14:34:29.609</t>
-  </si>
-  <si>
-    <t>14:34:16.771</t>
-  </si>
-  <si>
-    <t>14:34:40.455</t>
-  </si>
-  <si>
-    <t>14:34:16.025</t>
-  </si>
-  <si>
-    <t>14:34:47.988</t>
-  </si>
-  <si>
-    <t>14:34:15.293</t>
-  </si>
-  <si>
-    <t>14:34:49.360</t>
-  </si>
-  <si>
-    <t>14:34:14.745</t>
-  </si>
-  <si>
-    <t>14:34:53.926</t>
-  </si>
-  <si>
     <t>14:34:13.666</t>
   </si>
   <si>
     <t>14:34:58.559</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes de customer maintenance de la semana pasada aparecen exitosamente en pregame </t>
+  </si>
+  <si>
+    <t>13/11/2019</t>
+  </si>
+  <si>
+    <t>http://lobby.bminc.eu/</t>
+  </si>
+  <si>
+    <t>Chrome 78.0.3904.97</t>
+  </si>
+  <si>
+    <t>14:46:51.973</t>
+  </si>
+  <si>
+    <t>14:47:44.951</t>
+  </si>
+  <si>
+    <t>14/11/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 debería tener la configuración de zero balance Monday Zero Out pero tiene la siguiente configuración Tuesday Zero Out en su lugar </t>
+  </si>
+  <si>
+    <t>14:55:08.170</t>
+  </si>
+  <si>
+    <t>14:55:22.198</t>
+  </si>
+  <si>
+    <t>14:55:07.586</t>
+  </si>
+  <si>
+    <t>14:55:23.166</t>
+  </si>
+  <si>
+    <t>El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algún procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>14:55:06.780</t>
+  </si>
+  <si>
+    <t>14:55:23.834</t>
+  </si>
+  <si>
+    <t>15/11/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El monto de la transacciones del jugador PRAC06 del lunes de esta semana se ve reflejado correctamente en la semana pasada </t>
+  </si>
+  <si>
+    <t>El jugador "PRAC06" tiene la configración correcta de Tuesday Zero Out</t>
+  </si>
+  <si>
+    <t>15:03:11.870</t>
+  </si>
+  <si>
+    <t>15:03:36.232</t>
+  </si>
+  <si>
+    <t>15:03:41.753</t>
+  </si>
+  <si>
+    <t>15:03:44.698</t>
+  </si>
+  <si>
+    <t>15:03:41.291</t>
+  </si>
+  <si>
+    <t>15:03:53.930</t>
+  </si>
+  <si>
+    <t>15:03:40.505</t>
+  </si>
+  <si>
+    <t>15:04:01.127</t>
+  </si>
+  <si>
+    <t>15:03:39.801</t>
+  </si>
+  <si>
+    <t>15:04:02.480</t>
+  </si>
+  <si>
+    <t>15:03:39.128</t>
+  </si>
+  <si>
+    <t>15:04:07.086</t>
+  </si>
+  <si>
+    <t>15:03:10.763</t>
+  </si>
+  <si>
+    <t>15:04:11.035</t>
+  </si>
+  <si>
+    <t>15:05:49.659</t>
+  </si>
+  <si>
+    <t>15:06:18.347</t>
+  </si>
+  <si>
+    <t>15:06:23.650</t>
+  </si>
+  <si>
+    <t>15:06:26.480</t>
+  </si>
+  <si>
+    <t>15:06:23.221</t>
+  </si>
+  <si>
+    <t>15:06:37.964</t>
+  </si>
+  <si>
+    <t>15:06:22.516</t>
+  </si>
+  <si>
+    <t>15:06:45.670</t>
+  </si>
+  <si>
+    <t>15:06:21.770</t>
+  </si>
+  <si>
+    <t>15:06:46.898</t>
+  </si>
+  <si>
+    <t>15:06:21.124</t>
+  </si>
+  <si>
+    <t>15:06:51.461</t>
+  </si>
+  <si>
+    <t>15:05:48.701</t>
+  </si>
+  <si>
+    <t>15:06:55.351</t>
   </si>
 </sst>
 </file>
@@ -1684,25 +954,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
-        <v>392</v>
+        <v>147</v>
       </c>
       <c r="F2" t="s">
-        <v>393</v>
+        <v>148</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2137,25 +1407,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
-        <v>394</v>
+        <v>149</v>
       </c>
       <c r="F2" t="s">
-        <v>395</v>
+        <v>150</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2164,7 +1434,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2226,19 +1496,19 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>390</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>391</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -2857,25 +2127,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
-        <v>396</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>397</v>
+        <v>152</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3035,25 +2305,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
-        <v>398</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
-        <v>399</v>
+        <v>154</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3062,7 +2332,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3075,7 +2345,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,25 +2478,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>400</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
-        <v>401</v>
+        <v>110</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>229</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3235,7 +2505,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3245,9 +2515,9 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6562A8C0-FC7B-445D-A338-0FDEAA881DD7}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
@@ -3288,39 +2558,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
         <v>121</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>122</v>
-      </c>
-      <c r="D2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E2" t="s">
-        <v>387</v>
-      </c>
-      <c r="F2" t="s">
-        <v>388</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>389</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3406,6 +2676,170 @@
       </c>
       <c r="K2" t="s">
         <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED85A1E-5855-4828-AF8A-720EBAEB5BD6}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60E0AD5-252A-4476-8A18-E6411FD4D65A}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3514,6 +2948,261 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45C2F4C-9688-43A4-AFB0-202DB31C1257}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3191DE2E-BDD9-4F57-B738-D2A7FA9D3DED}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830D8FEC-E448-46DD-958F-4AC130B4257C}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L2"/>

</xml_diff>

<commit_message>
limpieza de casos de prueba del documento
</commit_message>
<xml_diff>
--- a/Data Files/TestData/Reports/TestResults.xlsx
+++ b/Data Files/TestData/Reports/TestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\QAPregameNuevo\Data Files\TestData\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B46410F-0848-45A5-81D2-F3E88B712E80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE54223-06F4-4006-8EB9-D1F1695AE457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="3060" windowWidth="21600" windowHeight="11385" firstSheet="21" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="3000" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C6414" sheetId="1" r:id="rId1"/>
@@ -44,14 +44,17 @@
     <sheet name="C6405" sheetId="29" r:id="rId29"/>
     <sheet name="C6402" sheetId="30" r:id="rId30"/>
     <sheet name="C6408" sheetId="31" r:id="rId31"/>
-    <sheet name="C6403" sheetId="32" r:id="rId32"/>
+    <sheet name="C6406" sheetId="34" r:id="rId32"/>
+    <sheet name="C6403" sheetId="32" r:id="rId33"/>
+    <sheet name="C6410" sheetId="33" r:id="rId34"/>
+    <sheet name="C6407" sheetId="35" r:id="rId35"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="367">
   <si>
     <t>URL</t>
   </si>
@@ -176,352 +179,982 @@
     <t>El botón de reportes de la sección "My Account" es visible</t>
   </si>
   <si>
+    <t>El botón pending aparece seleccionado de forma predeterminada correctamente</t>
+  </si>
+  <si>
+    <t>El boton de pending se ve correctamente</t>
+  </si>
+  <si>
+    <t>http://10.0.74.5/index/home</t>
+  </si>
+  <si>
+    <t>01/11/2019</t>
+  </si>
+  <si>
+    <t>4FKU01</t>
+  </si>
+  <si>
+    <t>10:26:02.579</t>
+  </si>
+  <si>
+    <t>10:27:21.291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El botón de pendings muestra existosamente que el jugador 4FKU01 no tiene apuestas pendientes </t>
+  </si>
+  <si>
+    <t>-HOE115</t>
+  </si>
+  <si>
+    <t>Ksvwbnk9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las apuestas 174739697-1,174739592-1,174739449-1  del jugador -HOE115 aparecen correctamente en la sección Pensdings de reprotes </t>
+  </si>
+  <si>
+    <t>-RI137</t>
+  </si>
+  <si>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>14:12:21.294</t>
+  </si>
+  <si>
+    <t>14:14:20.931</t>
+  </si>
+  <si>
+    <t>La prueba resulto fallida porque el jugador de prueba no tiene apuestas resueltas en customer maintenance, o algún componente que no pudó ser localizado.  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>15:00:56.135</t>
+  </si>
+  <si>
+    <t>15:01:30.571</t>
+  </si>
+  <si>
+    <t>15:00:55.444</t>
+  </si>
+  <si>
+    <t>15:01:33.558</t>
+  </si>
+  <si>
+    <t>15:00:27.986</t>
+  </si>
+  <si>
+    <t>15:01:36.339</t>
+  </si>
+  <si>
+    <t>4FKU100</t>
+  </si>
+  <si>
+    <t>15:44:46.030</t>
+  </si>
+  <si>
+    <t>15:45:07.526</t>
+  </si>
+  <si>
+    <t>15:44:45.367</t>
+  </si>
+  <si>
+    <t>15:45:08.566</t>
+  </si>
+  <si>
+    <t>Botón Graded es visible de forma satisfactoria</t>
+  </si>
+  <si>
+    <t>15:44:08.127</t>
+  </si>
+  <si>
+    <t>15:45:12.420</t>
+  </si>
+  <si>
+    <t>El sitio de pregame no muestra apuestas resueltas  del jugador 4FKU100 de forma exitosa</t>
+  </si>
+  <si>
+    <t>04/11/2019</t>
+  </si>
+  <si>
+    <t>09:24:38.273</t>
+  </si>
+  <si>
+    <t>09:24:42.110</t>
+  </si>
+  <si>
+    <t>09:24:43.490</t>
+  </si>
+  <si>
+    <t>09:24:46.862</t>
+  </si>
+  <si>
+    <t>09:24:48.334</t>
+  </si>
+  <si>
+    <t>09:24:57.023</t>
+  </si>
+  <si>
+    <t>09:24:58.477</t>
+  </si>
+  <si>
+    <t>09:25:08.285</t>
+  </si>
+  <si>
+    <t>09:25:11.769</t>
+  </si>
+  <si>
+    <t>09:25:19.551</t>
+  </si>
+  <si>
+    <t>09:25:23.585</t>
+  </si>
+  <si>
+    <t>09:25:30.812</t>
+  </si>
+  <si>
+    <t>El botón Daily Figure o Balance Diario de la sección "My Account" es visible</t>
+  </si>
+  <si>
+    <t>El combobox de semanas es visible</t>
+  </si>
+  <si>
+    <t>Chrome 78.0.3904.70</t>
+  </si>
+  <si>
+    <t>05/11/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El checkbox "Start From Tuesday" es visible correctamente </t>
+  </si>
+  <si>
+    <t>13:28:33.898</t>
+  </si>
+  <si>
+    <t>13:29:12.316</t>
+  </si>
+  <si>
+    <t>Permiso de Sportbook Deportes es correctamente accesible para el usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los días de la semana Lunes,Martes,Miércoles,Jueves,Viernes,Sábado,Domingo y  encabezado de sumatorial Total se ven correctamente en la tabla de días de la semana </t>
+  </si>
+  <si>
+    <t>El checkbox "Iniciar Martes" muestra correctamente los días de la semana con el siguiente orden: Martes,Miércoles,Jueves,Viernes,Sábado,Domingo,Lunes,Total</t>
+  </si>
+  <si>
+    <t>PRAC06</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Firefox 70.0.1</t>
+  </si>
+  <si>
+    <t>11/11/2019</t>
+  </si>
+  <si>
+    <t>14:34:13.666</t>
+  </si>
+  <si>
+    <t>14:34:58.559</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes de customer maintenance de la semana pasada aparecen exitosamente en pregame </t>
+  </si>
+  <si>
+    <t>13/11/2019</t>
+  </si>
+  <si>
+    <t>http://lobby.bminc.eu/</t>
+  </si>
+  <si>
+    <t>Chrome 78.0.3904.97</t>
+  </si>
+  <si>
+    <t>14:46:51.973</t>
+  </si>
+  <si>
+    <t>14:47:44.951</t>
+  </si>
+  <si>
+    <t>14/11/2019</t>
+  </si>
+  <si>
+    <t>14:55:06.780</t>
+  </si>
+  <si>
+    <t>14:55:23.834</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El monto de la transacciones del jugador PRAC06 del lunes de esta semana se ve reflejado correctamente en la semana pasada </t>
+  </si>
+  <si>
+    <t>16/11/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 debería tener la configuración de zero balance Monday Zero Out pero tiene la siguiente configuración Tuesday Zero Out en su lugar </t>
+  </si>
+  <si>
+    <t>12:14:39.111</t>
+  </si>
+  <si>
+    <t>12:15:02.812</t>
+  </si>
+  <si>
+    <t>12:14:37.959</t>
+  </si>
+  <si>
+    <t>12:15:05.178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algún procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09 o revisar el resultado de los siguientes casos de prueba [C6405] en el archivo exte de resultados de prueba para verificar si alguna precondición del casod e prueba fallo </t>
+  </si>
+  <si>
+    <t>12:23:58.162</t>
+  </si>
+  <si>
+    <t>12:24:11.086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 debería tener la configuración de zero balance Tuesday Zero Out pero tiene la siguiente configuración: Monday Zero Out en su lugar </t>
+  </si>
+  <si>
+    <t>El jugador "PRAC06" tiene la configración correcta de Tuesday Zero Out</t>
+  </si>
+  <si>
+    <t>12:58:09.949</t>
+  </si>
+  <si>
+    <t>12:58:25.071</t>
+  </si>
+  <si>
+    <t>12:58:28.553</t>
+  </si>
+  <si>
+    <t>12:59:00.753</t>
+  </si>
+  <si>
+    <t>12:58:08.964</t>
+  </si>
+  <si>
+    <t>12:59:04.839</t>
+  </si>
+  <si>
+    <t>12:56:25.493</t>
+  </si>
+  <si>
+    <t>12:59:33.834</t>
+  </si>
+  <si>
+    <t>15:18:01.875</t>
+  </si>
+  <si>
+    <t>15:18:28.300</t>
+  </si>
+  <si>
+    <t>15:18:00.529</t>
+  </si>
+  <si>
+    <t>15:18:35.770</t>
+  </si>
+  <si>
+    <t>15:17:59.321</t>
+  </si>
+  <si>
+    <t>15:18:37.334</t>
+  </si>
+  <si>
+    <t>15:17:58.397</t>
+  </si>
+  <si>
+    <t>15:18:39.327</t>
+  </si>
+  <si>
+    <t>15:17:57.210</t>
+  </si>
+  <si>
+    <t>15:19:21.110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La sumatoria de las transacciones diarias  del jugador PRAC06 son iguales al monto toal reflejado </t>
+  </si>
+  <si>
+    <t>19/11/2019</t>
+  </si>
+  <si>
+    <t>10:44:34.043</t>
+  </si>
+  <si>
+    <t>10:45:11.163</t>
+  </si>
+  <si>
+    <t>11:05:11.448</t>
+  </si>
+  <si>
+    <t>11:05:31.702</t>
+  </si>
+  <si>
+    <t>El sistema no pudo validar que el usuario no pueda entrar al sitio si su pin no es ingresado  debido a algún elemento de la pagina que no esta presente o fue modificado  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -01</t>
+  </si>
+  <si>
+    <t>El botón login debería ser visible, pero actualmente no lo es debido a un comportanmiento anomalo. Favor revisar el log de katalon con el código de error -99</t>
+  </si>
+  <si>
+    <t>El formaulrio de ingreso deberia ser visible, pero actualmente no lo es debido a un comportanmiento anomaloFavor de revisar en la consola de katalon con el siguiente código -99</t>
+  </si>
+  <si>
+    <t>11:05:38.434</t>
+  </si>
+  <si>
+    <t>11:05:39.510</t>
+  </si>
+  <si>
+    <t>11:05:37.140</t>
+  </si>
+  <si>
+    <t>11:05:40.761</t>
+  </si>
+  <si>
+    <t>11:13:07.032</t>
+  </si>
+  <si>
+    <t>11:13:23.796</t>
+  </si>
+  <si>
     <t>El botón login es visible</t>
   </si>
   <si>
-    <t>El botón pending aparece seleccionado de forma predeterminada correctamente</t>
-  </si>
-  <si>
-    <t>El boton de pending se ve correctamente</t>
-  </si>
-  <si>
-    <t>http://10.0.74.5/index/home</t>
-  </si>
-  <si>
-    <t>01/11/2019</t>
-  </si>
-  <si>
-    <t>4FKU01</t>
-  </si>
-  <si>
-    <t>10:26:02.579</t>
-  </si>
-  <si>
-    <t>10:27:21.291</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El botón de pendings muestra existosamente que el jugador 4FKU01 no tiene apuestas pendientes </t>
-  </si>
-  <si>
-    <t>-HOE115</t>
-  </si>
-  <si>
-    <t>Ksvwbnk9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las apuestas 174739697-1,174739592-1,174739449-1  del jugador -HOE115 aparecen correctamente en la sección Pensdings de reprotes </t>
-  </si>
-  <si>
-    <t>-RI137</t>
-  </si>
-  <si>
-    <t>Greg</t>
-  </si>
-  <si>
-    <t>14:12:21.294</t>
-  </si>
-  <si>
-    <t>14:14:20.931</t>
-  </si>
-  <si>
-    <t>La prueba resulto fallida porque el jugador de prueba no tiene apuestas resueltas en customer maintenance, o algún componente que no pudó ser localizado.  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
-  </si>
-  <si>
-    <t>15:00:56.135</t>
-  </si>
-  <si>
-    <t>15:01:30.571</t>
-  </si>
-  <si>
-    <t>15:00:55.444</t>
-  </si>
-  <si>
-    <t>15:01:33.558</t>
-  </si>
-  <si>
-    <t>15:00:27.986</t>
-  </si>
-  <si>
-    <t>15:01:36.339</t>
-  </si>
-  <si>
-    <t>4FKU100</t>
-  </si>
-  <si>
-    <t>15:44:46.030</t>
-  </si>
-  <si>
-    <t>15:45:07.526</t>
-  </si>
-  <si>
-    <t>15:44:45.367</t>
-  </si>
-  <si>
-    <t>15:45:08.566</t>
-  </si>
-  <si>
-    <t>Botón Graded es visible de forma satisfactoria</t>
-  </si>
-  <si>
-    <t>15:44:08.127</t>
-  </si>
-  <si>
-    <t>15:45:12.420</t>
-  </si>
-  <si>
-    <t>El sitio de pregame no muestra apuestas resueltas  del jugador 4FKU100 de forma exitosa</t>
-  </si>
-  <si>
-    <t>04/11/2019</t>
+    <t>11:13:06.572</t>
+  </si>
+  <si>
+    <t>11:13:27.992</t>
+  </si>
+  <si>
+    <t>El formulario de login es desplegado exitosamente con los siguientes campos:  User PIn or Email, Password,Remeber Credentials y botón &lt;Login&gt;</t>
+  </si>
+  <si>
+    <t>11:13:05.778</t>
+  </si>
+  <si>
+    <t>11:13:31.252</t>
   </si>
   <si>
     <t>El sistema no permitio que el usuario ingresará al sitio sin definir el pin de forma exitosa. El esperado mensaje de error 'The username or password is incorrect.' es desplegado existosamente</t>
   </si>
   <si>
-    <t>09:24:15.985</t>
-  </si>
-  <si>
-    <t>09:24:36.700</t>
-  </si>
-  <si>
-    <t>09:24:38.273</t>
-  </si>
-  <si>
-    <t>09:24:42.110</t>
-  </si>
-  <si>
-    <t>09:24:43.490</t>
-  </si>
-  <si>
-    <t>09:24:46.862</t>
-  </si>
-  <si>
-    <t>09:24:48.334</t>
-  </si>
-  <si>
-    <t>09:24:57.023</t>
-  </si>
-  <si>
-    <t>09:24:58.477</t>
-  </si>
-  <si>
-    <t>09:25:08.285</t>
-  </si>
-  <si>
-    <t>09:25:11.769</t>
-  </si>
-  <si>
-    <t>09:25:19.551</t>
-  </si>
-  <si>
-    <t>09:25:23.667</t>
-  </si>
-  <si>
-    <t>09:25:28.836</t>
-  </si>
-  <si>
-    <t>09:25:23.585</t>
-  </si>
-  <si>
-    <t>09:25:30.812</t>
-  </si>
-  <si>
-    <t>09:25:23.062</t>
-  </si>
-  <si>
-    <t>09:25:51.563</t>
-  </si>
-  <si>
-    <t>El botón Daily Figure o Balance Diario de la sección "My Account" es visible</t>
-  </si>
-  <si>
-    <t>El combobox de semanas es visible</t>
-  </si>
-  <si>
-    <t>Chrome 78.0.3904.70</t>
-  </si>
-  <si>
-    <t>13:46:24.421</t>
-  </si>
-  <si>
-    <t>13:47:00.979</t>
-  </si>
-  <si>
-    <t>05/11/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El checkbox "Start From Tuesday" es visible correctamente </t>
-  </si>
-  <si>
-    <t>13:28:33.898</t>
-  </si>
-  <si>
-    <t>13:29:12.316</t>
-  </si>
-  <si>
-    <t>Permiso de Sportbook Deportes es correctamente accesible para el usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los días de la semana Lunes,Martes,Miércoles,Jueves,Viernes,Sábado,Domingo y  encabezado de sumatorial Total se ven correctamente en la tabla de días de la semana </t>
-  </si>
-  <si>
-    <t>El checkbox "Iniciar Martes" muestra correctamente los días de la semana con el siguiente orden: Martes,Miércoles,Jueves,Viernes,Sábado,Domingo,Lunes,Total</t>
-  </si>
-  <si>
-    <t>PRAC06</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>Firefox 70.0.1</t>
-  </si>
-  <si>
-    <t>11/11/2019</t>
-  </si>
-  <si>
-    <t>14:34:13.666</t>
-  </si>
-  <si>
-    <t>14:34:58.559</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes de customer maintenance de la semana pasada aparecen exitosamente en pregame </t>
-  </si>
-  <si>
-    <t>13/11/2019</t>
-  </si>
-  <si>
-    <t>http://lobby.bminc.eu/</t>
-  </si>
-  <si>
-    <t>Chrome 78.0.3904.97</t>
-  </si>
-  <si>
-    <t>14:46:51.973</t>
-  </si>
-  <si>
-    <t>14:47:44.951</t>
-  </si>
-  <si>
-    <t>14/11/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El jugador PRAC06 debería tener la configuración de zero balance Monday Zero Out pero tiene la siguiente configuración Tuesday Zero Out en su lugar </t>
-  </si>
-  <si>
-    <t>14:55:08.170</t>
-  </si>
-  <si>
-    <t>14:55:22.198</t>
-  </si>
-  <si>
-    <t>14:55:07.586</t>
-  </si>
-  <si>
-    <t>14:55:23.166</t>
-  </si>
-  <si>
-    <t>El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algún procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
-  </si>
-  <si>
-    <t>14:55:06.780</t>
-  </si>
-  <si>
-    <t>14:55:23.834</t>
-  </si>
-  <si>
-    <t>15/11/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El monto de la transacciones del jugador PRAC06 del lunes de esta semana se ve reflejado correctamente en la semana pasada </t>
-  </si>
-  <si>
-    <t>El jugador "PRAC06" tiene la configración correcta de Tuesday Zero Out</t>
-  </si>
-  <si>
-    <t>15:03:11.870</t>
-  </si>
-  <si>
-    <t>15:03:36.232</t>
-  </si>
-  <si>
-    <t>15:03:41.753</t>
-  </si>
-  <si>
-    <t>15:03:44.698</t>
-  </si>
-  <si>
-    <t>15:03:41.291</t>
-  </si>
-  <si>
-    <t>15:03:53.930</t>
-  </si>
-  <si>
-    <t>15:03:40.505</t>
-  </si>
-  <si>
-    <t>15:04:01.127</t>
-  </si>
-  <si>
-    <t>15:03:39.801</t>
-  </si>
-  <si>
-    <t>15:04:02.480</t>
-  </si>
-  <si>
-    <t>15:03:39.128</t>
-  </si>
-  <si>
-    <t>15:04:07.086</t>
-  </si>
-  <si>
-    <t>15:03:10.763</t>
-  </si>
-  <si>
-    <t>15:04:11.035</t>
-  </si>
-  <si>
-    <t>15:05:49.659</t>
-  </si>
-  <si>
-    <t>15:06:18.347</t>
-  </si>
-  <si>
-    <t>15:06:23.650</t>
-  </si>
-  <si>
-    <t>15:06:26.480</t>
-  </si>
-  <si>
-    <t>15:06:23.221</t>
-  </si>
-  <si>
-    <t>15:06:37.964</t>
-  </si>
-  <si>
-    <t>15:06:22.516</t>
-  </si>
-  <si>
-    <t>15:06:45.670</t>
-  </si>
-  <si>
-    <t>15:06:21.770</t>
-  </si>
-  <si>
-    <t>15:06:46.898</t>
-  </si>
-  <si>
-    <t>15:06:21.124</t>
-  </si>
-  <si>
-    <t>15:06:51.461</t>
-  </si>
-  <si>
-    <t>15:05:48.701</t>
-  </si>
-  <si>
-    <t>15:06:55.351</t>
+    <t>11:17:39.203</t>
+  </si>
+  <si>
+    <t>11:17:52.298</t>
+  </si>
+  <si>
+    <t>11:17:38.600</t>
+  </si>
+  <si>
+    <t>11:17:56.027</t>
+  </si>
+  <si>
+    <t>11:17:37.675</t>
+  </si>
+  <si>
+    <t>11:17:59.310</t>
+  </si>
+  <si>
+    <t>11:18:01.353</t>
+  </si>
+  <si>
+    <t>11:18:01.452</t>
+  </si>
+  <si>
+    <t>11:18:01.242</t>
+  </si>
+  <si>
+    <t>11:18:03.267</t>
+  </si>
+  <si>
+    <t>11:18:01.139</t>
+  </si>
+  <si>
+    <t>11:18:05.567</t>
+  </si>
+  <si>
+    <t>11:18:07.423</t>
+  </si>
+  <si>
+    <t>11:18:07.538</t>
+  </si>
+  <si>
+    <t>11:18:07.311</t>
+  </si>
+  <si>
+    <t>11:18:09.288</t>
+  </si>
+  <si>
+    <t>11:18:07.217</t>
+  </si>
+  <si>
+    <t>11:18:14.605</t>
+  </si>
+  <si>
+    <t>11:18:16.061</t>
+  </si>
+  <si>
+    <t>11:18:26.412</t>
+  </si>
+  <si>
+    <t>El jugador logró ingresar al sitio de pregame con la tecla enter</t>
+  </si>
+  <si>
+    <t>12:21:41.960</t>
+  </si>
+  <si>
+    <t>12:21:54.312</t>
+  </si>
+  <si>
+    <t>12:21:41.433</t>
+  </si>
+  <si>
+    <t>12:21:58.128</t>
+  </si>
+  <si>
+    <t>12:21:40.593</t>
+  </si>
+  <si>
+    <t>12:22:01.467</t>
+  </si>
+  <si>
+    <t>12:22:03.302</t>
+  </si>
+  <si>
+    <t>12:22:03.435</t>
+  </si>
+  <si>
+    <t>12:22:03.191</t>
+  </si>
+  <si>
+    <t>12:22:05.202</t>
+  </si>
+  <si>
+    <t>12:22:03.082</t>
+  </si>
+  <si>
+    <t>12:22:07.653</t>
+  </si>
+  <si>
+    <t>12:22:09.494</t>
+  </si>
+  <si>
+    <t>12:22:09.622</t>
+  </si>
+  <si>
+    <t>12:22:09.368</t>
+  </si>
+  <si>
+    <t>12:22:11.441</t>
+  </si>
+  <si>
+    <t>12:22:09.192</t>
+  </si>
+  <si>
+    <t>12:22:17.831</t>
+  </si>
+  <si>
+    <t>12:22:19.815</t>
+  </si>
+  <si>
+    <t>12:22:26.194</t>
+  </si>
+  <si>
+    <t>12:22:19.677</t>
+  </si>
+  <si>
+    <t>12:22:28</t>
+  </si>
+  <si>
+    <t>12:22:19.581</t>
+  </si>
+  <si>
+    <t>12:22:35.312</t>
+  </si>
+  <si>
+    <t>12:22:43.038</t>
+  </si>
+  <si>
+    <t>12:22:43.132</t>
+  </si>
+  <si>
+    <t>12:22:36.908</t>
+  </si>
+  <si>
+    <t>12:22:44.838</t>
+  </si>
+  <si>
+    <t>12:22:36.814</t>
+  </si>
+  <si>
+    <t>12:22:53.474</t>
+  </si>
+  <si>
+    <t>12:23:00.284</t>
+  </si>
+  <si>
+    <t>12:23:00.396</t>
+  </si>
+  <si>
+    <t>12:22:54.835</t>
+  </si>
+  <si>
+    <t>12:23:08.771</t>
+  </si>
+  <si>
+    <t>12:22:54.750</t>
+  </si>
+  <si>
+    <t>12:23:29.502</t>
+  </si>
+  <si>
+    <t>12:26:44.323</t>
+  </si>
+  <si>
+    <t>12:27:09.846</t>
+  </si>
+  <si>
+    <t>El jugador "PRAC06" tiene la configración correcta de Monday Zero Out</t>
+  </si>
+  <si>
+    <t>12:26:43.329</t>
+  </si>
+  <si>
+    <t>12:27:17.276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algún procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09 o revisar el resultado de los siguientes casos de prueba [C6405] en el archivo excel de resultados de prueba para verificar si alguna precondición del caso de prueba falló </t>
+  </si>
+  <si>
+    <t>12:27:19.177</t>
+  </si>
+  <si>
+    <t>12:27:31.259</t>
+  </si>
+  <si>
+    <t>12:27:19.034</t>
+  </si>
+  <si>
+    <t>12:27:42.589</t>
+  </si>
+  <si>
+    <t>12:27:18.886</t>
+  </si>
+  <si>
+    <t>12:27:43.172</t>
+  </si>
+  <si>
+    <t>12:27:52.338</t>
+  </si>
+  <si>
+    <t>12:28:07.140</t>
+  </si>
+  <si>
+    <t>12:27:52.219</t>
+  </si>
+  <si>
+    <t>12:28:21.753</t>
+  </si>
+  <si>
+    <t>El jugador PRAC06 no tiene transacciones para el día lunes de la semana pasada o su configuración de zero balance no es del lunes o algón procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>http://sup-lobby.bminc.eu/index.php/pages/login#</t>
+  </si>
+  <si>
+    <t>12:33:55.452</t>
+  </si>
+  <si>
+    <t>12:34:27.172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador 4FKU100 debería tener la configuración de zero balance Monday Zero Out pero tiene la siguiente configuración Tuesday Zero Out en su lugar </t>
+  </si>
+  <si>
+    <t>12:33:54.092</t>
+  </si>
+  <si>
+    <t>12:34:30.769</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador 4FKU100 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algún procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09 o revisar el resultado de los siguientes casos de prueba [C6405] en el archivo excel de resultados de prueba para verificar si alguna precondición del caso de prueba falló </t>
+  </si>
+  <si>
+    <t>12:34:31.004</t>
+  </si>
+  <si>
+    <t>12:34:48.564</t>
+  </si>
+  <si>
+    <t>12:34:30.789</t>
+  </si>
+  <si>
+    <t>12:34:51.957</t>
+  </si>
+  <si>
+    <t>12:34:30.632</t>
+  </si>
+  <si>
+    <t>12:34:52.935</t>
+  </si>
+  <si>
+    <t>12:34:52.872</t>
+  </si>
+  <si>
+    <t>12:35:08.072</t>
+  </si>
+  <si>
+    <t>12:34:52.585</t>
+  </si>
+  <si>
+    <t>12:35:08.650</t>
+  </si>
+  <si>
+    <t>El jugador 4FKU100 no tiene transacciones para el día lunes de la semana pasada o su configuración de zero balance no es del lunes o algón procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>12:34:54.887</t>
+  </si>
+  <si>
+    <t>12:35:09.308</t>
+  </si>
+  <si>
+    <t>12:34:54.766</t>
+  </si>
+  <si>
+    <t>12:35:10.699</t>
+  </si>
+  <si>
+    <t>12:35:36.418</t>
+  </si>
+  <si>
+    <t>12:36:01.318</t>
+  </si>
+  <si>
+    <t>12:36:13.122</t>
+  </si>
+  <si>
+    <t>12:36:16.027</t>
+  </si>
+  <si>
+    <t>12:36:12.652</t>
+  </si>
+  <si>
+    <t>12:36:26.822</t>
+  </si>
+  <si>
+    <t>12:36:11.887</t>
+  </si>
+  <si>
+    <t>12:36:34.188</t>
+  </si>
+  <si>
+    <t>12:36:11.156</t>
+  </si>
+  <si>
+    <t>12:36:35.552</t>
+  </si>
+  <si>
+    <t>12:36:10.592</t>
+  </si>
+  <si>
+    <t>12:36:42.796</t>
+  </si>
+  <si>
+    <t>12:35:35.449</t>
+  </si>
+  <si>
+    <t>12:36:44.482</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes de customer maintenance aparecen exitosamente en pregame </t>
+  </si>
+  <si>
+    <t>12:36:54.303</t>
+  </si>
+  <si>
+    <t>12:36:55.050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El botón de  Iniciar Martes remueve las transacciones del día lunes del jugador PRAC06 existosamente  </t>
+  </si>
+  <si>
+    <t>12:36:59.957</t>
+  </si>
+  <si>
+    <t>12:37:12.396</t>
+  </si>
+  <si>
+    <t>12:36:55.897</t>
+  </si>
+  <si>
+    <t>12:37:17.789</t>
+  </si>
+  <si>
+    <t>13:09:32.965</t>
+  </si>
+  <si>
+    <t>13:09:58.171</t>
+  </si>
+  <si>
+    <t>13:10:10.005</t>
+  </si>
+  <si>
+    <t>13:10:12.895</t>
+  </si>
+  <si>
+    <t>13:10:09.581</t>
+  </si>
+  <si>
+    <t>13:10:23.290</t>
+  </si>
+  <si>
+    <t>13:10:08.823</t>
+  </si>
+  <si>
+    <t>13:10:30.463</t>
+  </si>
+  <si>
+    <t>13:10:08.066</t>
+  </si>
+  <si>
+    <t>13:10:31.727</t>
+  </si>
+  <si>
+    <t>13:10:07.395</t>
+  </si>
+  <si>
+    <t>13:10:39.796</t>
+  </si>
+  <si>
+    <t>13:09:32.042</t>
+  </si>
+  <si>
+    <t>13:10:41.538</t>
+  </si>
+  <si>
+    <t>13:10:51.499</t>
+  </si>
+  <si>
+    <t>13:10:52.306</t>
+  </si>
+  <si>
+    <t>13:11:02.003</t>
+  </si>
+  <si>
+    <t>13:11:14.982</t>
+  </si>
+  <si>
+    <t>13:10:53.073</t>
+  </si>
+  <si>
+    <t>13:11:27.958</t>
+  </si>
+  <si>
+    <t>13:13:13.809</t>
+  </si>
+  <si>
+    <t>13:13:52.440</t>
+  </si>
+  <si>
+    <t>13:17:40.153</t>
+  </si>
+  <si>
+    <t>13:18:04.457</t>
+  </si>
+  <si>
+    <t>13:17:39.172</t>
+  </si>
+  <si>
+    <t>13:18:09.523</t>
+  </si>
+  <si>
+    <t>13:19:59.134</t>
+  </si>
+  <si>
+    <t>13:20:25.105</t>
+  </si>
+  <si>
+    <t>13:19:58.218</t>
+  </si>
+  <si>
+    <t>13:21:01.320</t>
+  </si>
+  <si>
+    <t>13:23:18.615</t>
+  </si>
+  <si>
+    <t>13:23:43.399</t>
+  </si>
+  <si>
+    <t>13:23:17.825</t>
+  </si>
+  <si>
+    <t>13:24:19.716</t>
+  </si>
+  <si>
+    <t>13:28:53.499</t>
+  </si>
+  <si>
+    <t>13:29:21.160</t>
+  </si>
+  <si>
+    <t>13:28:51.632</t>
+  </si>
+  <si>
+    <t>13:29:29.308</t>
+  </si>
+  <si>
+    <t>13:32:40.976</t>
+  </si>
+  <si>
+    <t>13:33:06.535</t>
+  </si>
+  <si>
+    <t>13:32:39.911</t>
+  </si>
+  <si>
+    <t>13:33:12.292</t>
+  </si>
+  <si>
+    <t>La prueba no se pudo realizar debido a un fallo anomalo en la prueba Favor de revisar en la consola de katalon con el siguiente código -99</t>
+  </si>
+  <si>
+    <t>13:34:30.555</t>
+  </si>
+  <si>
+    <t>13:34:56.476</t>
+  </si>
+  <si>
+    <t>13:35:35.104</t>
+  </si>
+  <si>
+    <t>13:35:45.063</t>
+  </si>
+  <si>
+    <t>13:35:34.704</t>
+  </si>
+  <si>
+    <t>13:35:54.589</t>
+  </si>
+  <si>
+    <t>13:35:33.930</t>
+  </si>
+  <si>
+    <t>13:36:03.174</t>
+  </si>
+  <si>
+    <t>13:35:33.291</t>
+  </si>
+  <si>
+    <t>13:36:04.446</t>
+  </si>
+  <si>
+    <t>13:35:26.594</t>
+  </si>
+  <si>
+    <t>13:36:09.488</t>
+  </si>
+  <si>
+    <t>13:34:29.664</t>
+  </si>
+  <si>
+    <t>13:36:18.693</t>
+  </si>
+  <si>
+    <t>13:37:18.141</t>
+  </si>
+  <si>
+    <t>13:37:41.909</t>
+  </si>
+  <si>
+    <t>13:37:53.864</t>
+  </si>
+  <si>
+    <t>13:37:56.233</t>
+  </si>
+  <si>
+    <t>13:37:53.439</t>
+  </si>
+  <si>
+    <t>13:38:06.987</t>
+  </si>
+  <si>
+    <t>13:37:52.777</t>
+  </si>
+  <si>
+    <t>13:38:14.361</t>
+  </si>
+  <si>
+    <t>13:37:51.946</t>
+  </si>
+  <si>
+    <t>13:38:15.585</t>
+  </si>
+  <si>
+    <t>13:37:51.319</t>
+  </si>
+  <si>
+    <t>13:38:23.112</t>
+  </si>
+  <si>
+    <t>13:37:17.181</t>
+  </si>
+  <si>
+    <t>13:38:24.848</t>
+  </si>
+  <si>
+    <t>13:38:34.540</t>
+  </si>
+  <si>
+    <t>13:38:35.332</t>
+  </si>
+  <si>
+    <t>13:38:44.759</t>
+  </si>
+  <si>
+    <t>13:38:59.122</t>
+  </si>
+  <si>
+    <t>13:40:04.400</t>
+  </si>
+  <si>
+    <t>13:40:20.692</t>
+  </si>
+  <si>
+    <t>13:40:04.309</t>
+  </si>
+  <si>
+    <t>13:40:30.119</t>
+  </si>
+  <si>
+    <t>13:40:04.202</t>
+  </si>
+  <si>
+    <t>13:40:37.334</t>
+  </si>
+  <si>
+    <t>13:39:50.815</t>
+  </si>
+  <si>
+    <t>13:40:41.133</t>
+  </si>
+  <si>
+    <t>13:39:50.709</t>
+  </si>
+  <si>
+    <t>13:40:52.708</t>
+  </si>
+  <si>
+    <t>13:38:36.226</t>
+  </si>
+  <si>
+    <t>13:41:04.746</t>
   </si>
 </sst>
 </file>
@@ -954,25 +1587,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>357</v>
       </c>
       <c r="F2" t="s">
-        <v>148</v>
+        <v>358</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1040,25 +1673,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>217</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>218</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1125,19 +1758,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
         <v>65</v>
-      </c>
-      <c r="F2" t="s">
-        <v>66</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1218,22 +1851,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
       <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
         <v>58</v>
-      </c>
-      <c r="F2" t="s">
-        <v>59</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1248,7 +1881,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1310,22 +1943,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
       <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
         <v>60</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1340,7 +1973,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1407,25 +2040,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>359</v>
       </c>
       <c r="F2" t="s">
-        <v>150</v>
+        <v>360</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1434,7 +2067,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1496,19 +2129,19 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>355</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>356</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -1517,7 +2150,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1529,7 +2162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1570,19 +2205,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>215</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>216</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -1591,7 +2226,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1604,7 +2239,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,22 +2287,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
       <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
         <v>62</v>
-      </c>
-      <c r="F2" t="s">
-        <v>63</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1682,7 +2317,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1772,22 +2407,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1802,7 +2437,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1860,19 +2495,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
         <v>67</v>
-      </c>
-      <c r="F2" t="s">
-        <v>68</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1887,7 +2522,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1957,25 +2592,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2039,22 +2674,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>55</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2069,7 +2704,7 @@
         <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2082,7 +2717,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,25 +2762,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>151</v>
+        <v>361</v>
       </c>
       <c r="F2" t="s">
-        <v>152</v>
+        <v>362</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2154,7 +2789,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2220,25 +2855,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2247,7 +2882,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2305,25 +2940,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>363</v>
       </c>
       <c r="F2" t="s">
-        <v>154</v>
+        <v>364</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2332,7 +2967,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2390,28 +3025,28 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2420,7 +3055,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2478,25 +3113,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2505,7 +3140,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2518,7 +3153,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2563,34 +3198,34 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>349</v>
       </c>
       <c r="F2" t="s">
-        <v>122</v>
+        <v>350</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>123</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2648,19 +3283,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
         <v>70</v>
-      </c>
-      <c r="F2" t="s">
-        <v>71</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2675,7 +3310,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2733,25 +3368,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>365</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>366</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2760,7 +3395,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2812,34 +3447,34 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>353</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>354</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2851,8 +3486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,19 +3551,19 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>187</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2937,7 +3572,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
@@ -2998,34 +3633,34 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>351</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>352</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -3038,7 +3673,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3080,37 +3715,37 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="K2" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3119,11 +3754,11 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830D8FEC-E448-46DD-958F-4AC130B4257C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229C7116-4E07-47F6-B6A2-AA3E67FD8174}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3165,28 +3800,110 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830D8FEC-E448-46DD-958F-4AC130B4257C}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
         <v>126</v>
       </c>
-      <c r="E2" t="s">
-        <v>155</v>
-      </c>
       <c r="F2" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3195,7 +3912,177 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>127</v>
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{425D959C-196F-4131-A78D-F0B10FB4A717}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BA8E2D-405E-4E0A-8CFA-9B3F41877BEE}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3256,37 +4143,37 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>180</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>181</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3349,19 +4236,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -3438,25 +4325,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>206</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3523,25 +4410,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>211</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>212</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3616,19 +4503,19 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>194</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3689,13 +4576,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Correción de casos de prueba automatizados  de daily figure C6401,C3878,C6403,C3877,C6409
Mejora en el rendimiento de las pruebas automatizadas 

Signed-off-by: qa-katalon <qa-katalon@DEV-QA-KatalonStudio.BMinc.eu>
</commit_message>
<xml_diff>
--- a/Data Files/TestData/Reports/TestResults.xlsx
+++ b/Data Files/TestData/Reports/TestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\QAPregameNuevo\Data Files\TestData\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE54223-06F4-4006-8EB9-D1F1695AE457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF87160-B27D-4FA8-8CA6-3E079FE4AD48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="3000" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" firstSheet="28" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C6414" sheetId="1" r:id="rId1"/>
@@ -44,17 +44,21 @@
     <sheet name="C6405" sheetId="29" r:id="rId29"/>
     <sheet name="C6402" sheetId="30" r:id="rId30"/>
     <sheet name="C6408" sheetId="31" r:id="rId31"/>
-    <sheet name="C6406" sheetId="34" r:id="rId32"/>
-    <sheet name="C6403" sheetId="32" r:id="rId33"/>
-    <sheet name="C6410" sheetId="33" r:id="rId34"/>
+    <sheet name="C6403" sheetId="32" r:id="rId32"/>
+    <sheet name="C6406" sheetId="33" r:id="rId33"/>
+    <sheet name="C6410" sheetId="34" r:id="rId34"/>
     <sheet name="C6407" sheetId="35" r:id="rId35"/>
+    <sheet name="C3877" sheetId="36" r:id="rId36"/>
+    <sheet name="C6409" sheetId="37" r:id="rId37"/>
+    <sheet name="C3878" sheetId="38" r:id="rId38"/>
+    <sheet name="Sheet4" sheetId="39" r:id="rId39"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2618" uniqueCount="530">
   <si>
     <t>URL</t>
   </si>
@@ -179,6 +183,9 @@
     <t>El botón de reportes de la sección "My Account" es visible</t>
   </si>
   <si>
+    <t>El botón login es visible</t>
+  </si>
+  <si>
     <t>El botón pending aparece seleccionado de forma predeterminada correctamente</t>
   </si>
   <si>
@@ -275,6 +282,15 @@
     <t>04/11/2019</t>
   </si>
   <si>
+    <t>El sistema no permitio que el usuario ingresará al sitio sin definir el pin de forma exitosa. El esperado mensaje de error 'The username or password is incorrect.' es desplegado existosamente</t>
+  </si>
+  <si>
+    <t>09:24:15.985</t>
+  </si>
+  <si>
+    <t>09:24:36.700</t>
+  </si>
+  <si>
     <t>09:24:38.273</t>
   </si>
   <si>
@@ -305,12 +321,24 @@
     <t>09:25:19.551</t>
   </si>
   <si>
+    <t>09:25:23.667</t>
+  </si>
+  <si>
+    <t>09:25:28.836</t>
+  </si>
+  <si>
     <t>09:25:23.585</t>
   </si>
   <si>
     <t>09:25:30.812</t>
   </si>
   <si>
+    <t>09:25:23.062</t>
+  </si>
+  <si>
+    <t>09:25:51.563</t>
+  </si>
+  <si>
     <t>El botón Daily Figure o Balance Diario de la sección "My Account" es visible</t>
   </si>
   <si>
@@ -359,802 +387,1267 @@
     <t>14:34:58.559</t>
   </si>
   <si>
+    <t>http://lobby.bminc.eu/</t>
+  </si>
+  <si>
+    <t>Chrome 78.0.3904.97</t>
+  </si>
+  <si>
+    <t>15/11/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El monto de la transacciones del jugador PRAC06 del lunes de esta semana se ve reflejado correctamente en la semana pasada </t>
+  </si>
+  <si>
+    <t>El jugador "PRAC06" tiene la configración correcta de Tuesday Zero Out</t>
+  </si>
+  <si>
+    <t>15:05:49.659</t>
+  </si>
+  <si>
+    <t>15:06:18.347</t>
+  </si>
+  <si>
+    <t>21/11/2019</t>
+  </si>
+  <si>
+    <t>El jugador "PRAC06" tiene la configración correcta de Monday Zero Out</t>
+  </si>
+  <si>
+    <t>El jugador PRAC06 no tiene transacciones para el día lunes de la semana pasada o su configuración de zero balance no es del lunes o algón procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes de customer maintenance aparecen exitosamente en pregame </t>
+  </si>
+  <si>
+    <t>09:06:15.957</t>
+  </si>
+  <si>
+    <t>09:08:30.778</t>
+  </si>
+  <si>
+    <t>09:08:32.885</t>
+  </si>
+  <si>
+    <t>09:08:50.561</t>
+  </si>
+  <si>
+    <t>09:08:58.621</t>
+  </si>
+  <si>
+    <t>09:09:46.362</t>
+  </si>
+  <si>
+    <t>09:08:32.761</t>
+  </si>
+  <si>
+    <t>09:09:58.601</t>
+  </si>
+  <si>
+    <t>09:08:32.650</t>
+  </si>
+  <si>
+    <t>09:09:59.460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El botón de  Iniciar Martes remueve las transacciones del día lunes del jugador PRAC06 existosamente  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 debería tener la configuración de zero balance Tuesday Zero Out pero tiene la siguiente configuración: Monday Zero Out en su lugar </t>
+  </si>
+  <si>
+    <t>09:17:03.232</t>
+  </si>
+  <si>
+    <t>09:17:21.977</t>
+  </si>
+  <si>
+    <t>09:17:02.574</t>
+  </si>
+  <si>
+    <t>09:17:24.950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El monto de la transacciones del jugador PRAC06 del lunes de esta semana no se ve reflejado correctamente en la semana pasada Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  C6403-09 o revisar el resultado de los siguientes casos de prueba [C6406] en el archivo excel de resultados de prueba para verificar si alguna precondición del caso de prueba falló </t>
+  </si>
+  <si>
+    <t>09:16:36.359</t>
+  </si>
+  <si>
+    <t>09:17:26.075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 no tiene transacciones para el día lunes de la semana pasada   Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09 o revisar el resultado de los siguientes casos de prueba [C6403] en el archivo excel de resultados de prueba para verificar si alguna precondición del caso de prueba falló </t>
+  </si>
+  <si>
+    <t>09:20:45.397</t>
+  </si>
+  <si>
+    <t>09:20:58.823</t>
+  </si>
+  <si>
+    <t>09:20:44.969</t>
+  </si>
+  <si>
+    <t>09:21:11.618</t>
+  </si>
+  <si>
+    <t>09:20:44.235</t>
+  </si>
+  <si>
+    <t>09:21:19.125</t>
+  </si>
+  <si>
+    <t>09:20:42.871</t>
+  </si>
+  <si>
+    <t>09:21:20.574</t>
+  </si>
+  <si>
+    <t>09:20:42.140</t>
+  </si>
+  <si>
+    <t>09:21:22.321</t>
+  </si>
+  <si>
+    <t>09:20:41.095</t>
+  </si>
+  <si>
+    <t>09:21:26.549</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La sumatoria de las transacciones diarias  del jugador PRAC06 son iguales al monto total reflejado </t>
+  </si>
+  <si>
+    <t>22/11/2019</t>
+  </si>
+  <si>
+    <t>10:25:54.279</t>
+  </si>
+  <si>
+    <t>10:25:54.616</t>
+  </si>
+  <si>
+    <t>La prueba no se pudo realizar debido a un fallo anomalo en la prueba Favor de revisar en la consola de katalon con el siguiente código C3877-99</t>
+  </si>
+  <si>
+    <t>10:30:18.272</t>
+  </si>
+  <si>
+    <t>10:30:31.596</t>
+  </si>
+  <si>
+    <t>10:30:17.805</t>
+  </si>
+  <si>
+    <t>10:30:43.987</t>
+  </si>
+  <si>
+    <t>10:30:17.157</t>
+  </si>
+  <si>
+    <t>10:30:51.379</t>
+  </si>
+  <si>
+    <t>10:30:07.448</t>
+  </si>
+  <si>
+    <t>10:30:52.939</t>
+  </si>
+  <si>
+    <t>10:30:06.903</t>
+  </si>
+  <si>
+    <t>10:30:57.203</t>
+  </si>
+  <si>
+    <t>10:28:55.222</t>
+  </si>
+  <si>
+    <t>10:31:40.340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 no tiene transacciones para el día martes de la semana pasada o su configuración de zero balance no es del martes o algón procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09 o revisar el resultado de los siguientes casos de prueba [C6406] en el archivo excel de resultados de prueba para verificar si alguna precondición del caso de prueba falló </t>
+  </si>
+  <si>
+    <t>10:35:12.292</t>
+  </si>
+  <si>
+    <t>10:35:28.182</t>
+  </si>
+  <si>
+    <t>10:35:11.849</t>
+  </si>
+  <si>
+    <t>10:35:43.703</t>
+  </si>
+  <si>
+    <t>10:35:11.192</t>
+  </si>
+  <si>
+    <t>10:35:50.919</t>
+  </si>
+  <si>
+    <t>10:34:56.711</t>
+  </si>
+  <si>
+    <t>10:35:53.251</t>
+  </si>
+  <si>
+    <t>10:34:56.172</t>
+  </si>
+  <si>
+    <t>10:36:02.843</t>
+  </si>
+  <si>
+    <t>10:33:39.331</t>
+  </si>
+  <si>
+    <t>10:36:46.200</t>
+  </si>
+  <si>
+    <t>10:41:46.863</t>
+  </si>
+  <si>
+    <t>10:42:03.378</t>
+  </si>
+  <si>
+    <t>10:41:46.416</t>
+  </si>
+  <si>
+    <t>10:42:18.261</t>
+  </si>
+  <si>
+    <t>10:41:45.726</t>
+  </si>
+  <si>
+    <t>10:42:25.823</t>
+  </si>
+  <si>
+    <t>10:41:30.646</t>
+  </si>
+  <si>
+    <t>10:42:29.490</t>
+  </si>
+  <si>
+    <t>10:41:30.122</t>
+  </si>
+  <si>
+    <t>10:42:39.533</t>
+  </si>
+  <si>
+    <t>10:40:13.656</t>
+  </si>
+  <si>
+    <t>10:42:42.459</t>
+  </si>
+  <si>
+    <t>La prueba no se pudo realizar debido a un fallo anomalo en la prueba Favor de revisar en la consola de katalon con el siguiente código -99</t>
+  </si>
+  <si>
+    <t>10:47:03.357</t>
+  </si>
+  <si>
+    <t>10:47:06.360</t>
+  </si>
+  <si>
+    <t>10:49:37.428</t>
+  </si>
+  <si>
+    <t>10:49:56.305</t>
+  </si>
+  <si>
+    <t>10:49:36.944</t>
+  </si>
+  <si>
+    <t>10:50:08.454</t>
+  </si>
+  <si>
+    <t>10:49:36.205</t>
+  </si>
+  <si>
+    <t>10:50:15.984</t>
+  </si>
+  <si>
+    <t>10:49:21.331</t>
+  </si>
+  <si>
+    <t>10:50:20.139</t>
+  </si>
+  <si>
+    <t>10:49:20.764</t>
+  </si>
+  <si>
+    <t>10:50:30.588</t>
+  </si>
+  <si>
+    <t>10:48:05.770</t>
+  </si>
+  <si>
+    <t>10:51:20.705</t>
+  </si>
+  <si>
+    <t>12:07:34.766</t>
+  </si>
+  <si>
+    <t>12:07:37.709</t>
+  </si>
+  <si>
+    <t>12:07:32.853</t>
+  </si>
+  <si>
+    <t>12:07:50.974</t>
+  </si>
+  <si>
+    <t>12:07:32.039</t>
+  </si>
+  <si>
+    <t>12:07:58.305</t>
+  </si>
+  <si>
+    <t>12:07:31.354</t>
+  </si>
+  <si>
+    <t>12:07:59.813</t>
+  </si>
+  <si>
+    <t>12:07:30.313</t>
+  </si>
+  <si>
+    <t>12:08:04.350</t>
+  </si>
+  <si>
+    <t>12:06:52.812</t>
+  </si>
+  <si>
+    <t>12:08:46.475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 no tiene transacciones para el día lunes de la semana ante pasada o su configuración de zero balance no es del lunes o algón procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  C3878-09 o revisar el resultado de los siguientes casos de prueba [C6405] en el archivo excel de resultados de prueba para verificar si alguna precondición del caso de prueba falló </t>
+  </si>
+  <si>
+    <t>12:43:09.462</t>
+  </si>
+  <si>
+    <t>12:43:13.682</t>
+  </si>
+  <si>
+    <t>12:43:08.982</t>
+  </si>
+  <si>
+    <t>12:43:25.691</t>
+  </si>
+  <si>
+    <t>12:43:08.171</t>
+  </si>
+  <si>
+    <t>12:43:33.022</t>
+  </si>
+  <si>
+    <t>12:43:07.532</t>
+  </si>
+  <si>
+    <t>12:43:34.468</t>
+  </si>
+  <si>
+    <t>12:43:06.110</t>
+  </si>
+  <si>
+    <t>12:43:38.691</t>
+  </si>
+  <si>
+    <t>12:42:26.650</t>
+  </si>
+  <si>
+    <t>12:43:41.497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes de customer maintenance de la semana ante pasada aparecen exitosamente en pregame </t>
+  </si>
+  <si>
+    <t>12:49:00.091</t>
+  </si>
+  <si>
+    <t>12:49:12.790</t>
+  </si>
+  <si>
+    <t>12:48:59.597</t>
+  </si>
+  <si>
+    <t>12:49:25.500</t>
+  </si>
+  <si>
+    <t>12:48:58.762</t>
+  </si>
+  <si>
+    <t>12:49:33.138</t>
+  </si>
+  <si>
+    <t>12:48:57.964</t>
+  </si>
+  <si>
+    <t>12:49:34.500</t>
+  </si>
+  <si>
+    <t>12:48:57.341</t>
+  </si>
+  <si>
+    <t>12:49:39.077</t>
+  </si>
+  <si>
+    <t>12:48:56.368</t>
+  </si>
+  <si>
+    <t>12:49:43.271</t>
+  </si>
+  <si>
+    <t>12:51:22.078</t>
+  </si>
+  <si>
+    <t>12:51:23.024</t>
+  </si>
+  <si>
+    <t>12:52:32.062</t>
+  </si>
+  <si>
+    <t>12:52:36.699</t>
+  </si>
+  <si>
+    <t>Chrome 78.0.3904.108</t>
+  </si>
+  <si>
+    <t>12:52:31.610</t>
+  </si>
+  <si>
+    <t>12:52:51.383</t>
+  </si>
+  <si>
+    <t>12:52:30.865</t>
+  </si>
+  <si>
+    <t>12:52:58.690</t>
+  </si>
+  <si>
+    <t>12:52:30.197</t>
+  </si>
+  <si>
+    <t>12:53:00.152</t>
+  </si>
+  <si>
+    <t>12:52:29.603</t>
+  </si>
+  <si>
+    <t>12:53:04.557</t>
+  </si>
+  <si>
+    <t>12:52:28.986</t>
+  </si>
+  <si>
+    <t>12:53:08.780</t>
+  </si>
+  <si>
+    <t>12:51:56.694</t>
+  </si>
+  <si>
+    <t>12:53:12.560</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día martes de customer maintenance aparecen exitosamente en pregame </t>
+  </si>
+  <si>
+    <t>12:55:33.241</t>
+  </si>
+  <si>
+    <t>12:55:35.537</t>
+  </si>
+  <si>
+    <t>12:56:19.122</t>
+  </si>
+  <si>
+    <t>12:56:21.480</t>
+  </si>
+  <si>
+    <t>12:58:06.147</t>
+  </si>
+  <si>
+    <t>12:58:09.764</t>
+  </si>
+  <si>
+    <t>12:58:02.764</t>
+  </si>
+  <si>
+    <t>12:58:22.040</t>
+  </si>
+  <si>
+    <t>12:58:02.050</t>
+  </si>
+  <si>
+    <t>12:58:29.548</t>
+  </si>
+  <si>
+    <t>12:58:01.412</t>
+  </si>
+  <si>
+    <t>12:58:31.490</t>
+  </si>
+  <si>
+    <t>12:58:00.828</t>
+  </si>
+  <si>
+    <t>12:58:35.983</t>
+  </si>
+  <si>
+    <t>12:57:08.507</t>
+  </si>
+  <si>
+    <t>12:58:40.726</t>
+  </si>
+  <si>
     <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes de customer maintenance de la semana pasada aparecen exitosamente en pregame </t>
   </si>
   <si>
-    <t>13/11/2019</t>
-  </si>
-  <si>
-    <t>http://lobby.bminc.eu/</t>
-  </si>
-  <si>
-    <t>Chrome 78.0.3904.97</t>
-  </si>
-  <si>
-    <t>14:46:51.973</t>
-  </si>
-  <si>
-    <t>14:47:44.951</t>
-  </si>
-  <si>
-    <t>14/11/2019</t>
-  </si>
-  <si>
-    <t>14:55:06.780</t>
-  </si>
-  <si>
-    <t>14:55:23.834</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El monto de la transacciones del jugador PRAC06 del lunes de esta semana se ve reflejado correctamente en la semana pasada </t>
-  </si>
-  <si>
-    <t>16/11/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El jugador PRAC06 debería tener la configuración de zero balance Monday Zero Out pero tiene la siguiente configuración Tuesday Zero Out en su lugar </t>
-  </si>
-  <si>
-    <t>12:14:39.111</t>
-  </si>
-  <si>
-    <t>12:15:02.812</t>
-  </si>
-  <si>
-    <t>12:14:37.959</t>
-  </si>
-  <si>
-    <t>12:15:05.178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algún procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09 o revisar el resultado de los siguientes casos de prueba [C6405] en el archivo exte de resultados de prueba para verificar si alguna precondición del casod e prueba fallo </t>
-  </si>
-  <si>
-    <t>12:23:58.162</t>
-  </si>
-  <si>
-    <t>12:24:11.086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El jugador PRAC06 debería tener la configuración de zero balance Tuesday Zero Out pero tiene la siguiente configuración: Monday Zero Out en su lugar </t>
-  </si>
-  <si>
-    <t>El jugador "PRAC06" tiene la configración correcta de Tuesday Zero Out</t>
-  </si>
-  <si>
-    <t>12:58:09.949</t>
-  </si>
-  <si>
-    <t>12:58:25.071</t>
-  </si>
-  <si>
-    <t>12:58:28.553</t>
-  </si>
-  <si>
-    <t>12:59:00.753</t>
-  </si>
-  <si>
-    <t>12:58:08.964</t>
-  </si>
-  <si>
-    <t>12:59:04.839</t>
-  </si>
-  <si>
-    <t>12:56:25.493</t>
-  </si>
-  <si>
-    <t>12:59:33.834</t>
-  </si>
-  <si>
-    <t>15:18:01.875</t>
-  </si>
-  <si>
-    <t>15:18:28.300</t>
-  </si>
-  <si>
-    <t>15:18:00.529</t>
-  </si>
-  <si>
-    <t>15:18:35.770</t>
-  </si>
-  <si>
-    <t>15:17:59.321</t>
-  </si>
-  <si>
-    <t>15:18:37.334</t>
-  </si>
-  <si>
-    <t>15:17:58.397</t>
-  </si>
-  <si>
-    <t>15:18:39.327</t>
-  </si>
-  <si>
-    <t>15:17:57.210</t>
-  </si>
-  <si>
-    <t>15:19:21.110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La sumatoria de las transacciones diarias  del jugador PRAC06 son iguales al monto toal reflejado </t>
-  </si>
-  <si>
-    <t>19/11/2019</t>
-  </si>
-  <si>
-    <t>10:44:34.043</t>
-  </si>
-  <si>
-    <t>10:45:11.163</t>
-  </si>
-  <si>
-    <t>11:05:11.448</t>
-  </si>
-  <si>
-    <t>11:05:31.702</t>
-  </si>
-  <si>
-    <t>El sistema no pudo validar que el usuario no pueda entrar al sitio si su pin no es ingresado  debido a algún elemento de la pagina que no esta presente o fue modificado  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -01</t>
-  </si>
-  <si>
-    <t>El botón login debería ser visible, pero actualmente no lo es debido a un comportanmiento anomalo. Favor revisar el log de katalon con el código de error -99</t>
-  </si>
-  <si>
-    <t>El formaulrio de ingreso deberia ser visible, pero actualmente no lo es debido a un comportanmiento anomaloFavor de revisar en la consola de katalon con el siguiente código -99</t>
-  </si>
-  <si>
-    <t>11:05:38.434</t>
-  </si>
-  <si>
-    <t>11:05:39.510</t>
-  </si>
-  <si>
-    <t>11:05:37.140</t>
-  </si>
-  <si>
-    <t>11:05:40.761</t>
-  </si>
-  <si>
-    <t>11:13:07.032</t>
-  </si>
-  <si>
-    <t>11:13:23.796</t>
-  </si>
-  <si>
-    <t>El botón login es visible</t>
-  </si>
-  <si>
-    <t>11:13:06.572</t>
-  </si>
-  <si>
-    <t>11:13:27.992</t>
+    <t>13:07:20.675</t>
+  </si>
+  <si>
+    <t>13:07:34.088</t>
+  </si>
+  <si>
+    <t>13:07:19.925</t>
+  </si>
+  <si>
+    <t>13:07:46.557</t>
+  </si>
+  <si>
+    <t>13:11:47.975</t>
+  </si>
+  <si>
+    <t>13:12:01.214</t>
+  </si>
+  <si>
+    <t>13:11:47.380</t>
+  </si>
+  <si>
+    <t>13:12:13.317</t>
+  </si>
+  <si>
+    <t>13:13:21.957</t>
+  </si>
+  <si>
+    <t>13:13:35.420</t>
+  </si>
+  <si>
+    <t>13:14:30.916</t>
+  </si>
+  <si>
+    <t>13:14:45.790</t>
+  </si>
+  <si>
+    <t>13:14:30.222</t>
+  </si>
+  <si>
+    <t>13:14:55.752</t>
+  </si>
+  <si>
+    <t>13:19:01.132</t>
+  </si>
+  <si>
+    <t>13:19:13.936</t>
+  </si>
+  <si>
+    <t>13:19:00.270</t>
+  </si>
+  <si>
+    <t>13:19:18.070</t>
   </si>
   <si>
     <t>El formulario de login es desplegado exitosamente con los siguientes campos:  User PIn or Email, Password,Remeber Credentials y botón &lt;Login&gt;</t>
   </si>
   <si>
-    <t>11:13:05.778</t>
-  </si>
-  <si>
-    <t>11:13:31.252</t>
-  </si>
-  <si>
-    <t>El sistema no permitio que el usuario ingresará al sitio sin definir el pin de forma exitosa. El esperado mensaje de error 'The username or password is incorrect.' es desplegado existosamente</t>
-  </si>
-  <si>
-    <t>11:17:39.203</t>
-  </si>
-  <si>
-    <t>11:17:52.298</t>
-  </si>
-  <si>
-    <t>11:17:38.600</t>
-  </si>
-  <si>
-    <t>11:17:56.027</t>
-  </si>
-  <si>
-    <t>11:17:37.675</t>
-  </si>
-  <si>
-    <t>11:17:59.310</t>
-  </si>
-  <si>
-    <t>11:18:01.353</t>
-  </si>
-  <si>
-    <t>11:18:01.452</t>
-  </si>
-  <si>
-    <t>11:18:01.242</t>
-  </si>
-  <si>
-    <t>11:18:03.267</t>
-  </si>
-  <si>
-    <t>11:18:01.139</t>
-  </si>
-  <si>
-    <t>11:18:05.567</t>
-  </si>
-  <si>
-    <t>11:18:07.423</t>
-  </si>
-  <si>
-    <t>11:18:07.538</t>
-  </si>
-  <si>
-    <t>11:18:07.311</t>
-  </si>
-  <si>
-    <t>11:18:09.288</t>
-  </si>
-  <si>
-    <t>11:18:07.217</t>
-  </si>
-  <si>
-    <t>11:18:14.605</t>
-  </si>
-  <si>
-    <t>11:18:16.061</t>
-  </si>
-  <si>
-    <t>11:18:26.412</t>
-  </si>
-  <si>
-    <t>El jugador logró ingresar al sitio de pregame con la tecla enter</t>
-  </si>
-  <si>
-    <t>12:21:41.960</t>
-  </si>
-  <si>
-    <t>12:21:54.312</t>
-  </si>
-  <si>
-    <t>12:21:41.433</t>
-  </si>
-  <si>
-    <t>12:21:58.128</t>
-  </si>
-  <si>
-    <t>12:21:40.593</t>
-  </si>
-  <si>
-    <t>12:22:01.467</t>
-  </si>
-  <si>
-    <t>12:22:03.302</t>
-  </si>
-  <si>
-    <t>12:22:03.435</t>
-  </si>
-  <si>
-    <t>12:22:03.191</t>
-  </si>
-  <si>
-    <t>12:22:05.202</t>
-  </si>
-  <si>
-    <t>12:22:03.082</t>
-  </si>
-  <si>
-    <t>12:22:07.653</t>
-  </si>
-  <si>
-    <t>12:22:09.494</t>
-  </si>
-  <si>
-    <t>12:22:09.622</t>
-  </si>
-  <si>
-    <t>12:22:09.368</t>
-  </si>
-  <si>
-    <t>12:22:11.441</t>
-  </si>
-  <si>
-    <t>12:22:09.192</t>
-  </si>
-  <si>
-    <t>12:22:17.831</t>
-  </si>
-  <si>
-    <t>12:22:19.815</t>
-  </si>
-  <si>
-    <t>12:22:26.194</t>
-  </si>
-  <si>
-    <t>12:22:19.677</t>
-  </si>
-  <si>
-    <t>12:22:28</t>
-  </si>
-  <si>
-    <t>12:22:19.581</t>
-  </si>
-  <si>
-    <t>12:22:35.312</t>
-  </si>
-  <si>
-    <t>12:22:43.038</t>
-  </si>
-  <si>
-    <t>12:22:43.132</t>
-  </si>
-  <si>
-    <t>12:22:36.908</t>
-  </si>
-  <si>
-    <t>12:22:44.838</t>
-  </si>
-  <si>
-    <t>12:22:36.814</t>
-  </si>
-  <si>
-    <t>12:22:53.474</t>
-  </si>
-  <si>
-    <t>12:23:00.284</t>
-  </si>
-  <si>
-    <t>12:23:00.396</t>
-  </si>
-  <si>
-    <t>12:22:54.835</t>
-  </si>
-  <si>
-    <t>12:23:08.771</t>
-  </si>
-  <si>
-    <t>12:22:54.750</t>
-  </si>
-  <si>
-    <t>12:23:29.502</t>
-  </si>
-  <si>
-    <t>12:26:44.323</t>
-  </si>
-  <si>
-    <t>12:27:09.846</t>
-  </si>
-  <si>
-    <t>El jugador "PRAC06" tiene la configración correcta de Monday Zero Out</t>
-  </si>
-  <si>
-    <t>12:26:43.329</t>
-  </si>
-  <si>
-    <t>12:27:17.276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algún procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09 o revisar el resultado de los siguientes casos de prueba [C6405] en el archivo excel de resultados de prueba para verificar si alguna precondición del caso de prueba falló </t>
-  </si>
-  <si>
-    <t>12:27:19.177</t>
-  </si>
-  <si>
-    <t>12:27:31.259</t>
-  </si>
-  <si>
-    <t>12:27:19.034</t>
-  </si>
-  <si>
-    <t>12:27:42.589</t>
-  </si>
-  <si>
-    <t>12:27:18.886</t>
-  </si>
-  <si>
-    <t>12:27:43.172</t>
-  </si>
-  <si>
-    <t>12:27:52.338</t>
-  </si>
-  <si>
-    <t>12:28:07.140</t>
-  </si>
-  <si>
-    <t>12:27:52.219</t>
-  </si>
-  <si>
-    <t>12:28:21.753</t>
-  </si>
-  <si>
-    <t>El jugador PRAC06 no tiene transacciones para el día lunes de la semana pasada o su configuración de zero balance no es del lunes o algón procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
-  </si>
-  <si>
-    <t>http://sup-lobby.bminc.eu/index.php/pages/login#</t>
-  </si>
-  <si>
-    <t>12:33:55.452</t>
-  </si>
-  <si>
-    <t>12:34:27.172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El jugador 4FKU100 debería tener la configuración de zero balance Monday Zero Out pero tiene la siguiente configuración Tuesday Zero Out en su lugar </t>
-  </si>
-  <si>
-    <t>12:33:54.092</t>
-  </si>
-  <si>
-    <t>12:34:30.769</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El jugador 4FKU100 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algún procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09 o revisar el resultado de los siguientes casos de prueba [C6405] en el archivo excel de resultados de prueba para verificar si alguna precondición del caso de prueba falló </t>
-  </si>
-  <si>
-    <t>12:34:31.004</t>
-  </si>
-  <si>
-    <t>12:34:48.564</t>
-  </si>
-  <si>
-    <t>12:34:30.789</t>
-  </si>
-  <si>
-    <t>12:34:51.957</t>
-  </si>
-  <si>
-    <t>12:34:30.632</t>
-  </si>
-  <si>
-    <t>12:34:52.935</t>
-  </si>
-  <si>
-    <t>12:34:52.872</t>
-  </si>
-  <si>
-    <t>12:35:08.072</t>
-  </si>
-  <si>
-    <t>12:34:52.585</t>
-  </si>
-  <si>
-    <t>12:35:08.650</t>
-  </si>
-  <si>
-    <t>El jugador 4FKU100 no tiene transacciones para el día lunes de la semana pasada o su configuración de zero balance no es del lunes o algón procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
-  </si>
-  <si>
-    <t>12:34:54.887</t>
-  </si>
-  <si>
-    <t>12:35:09.308</t>
-  </si>
-  <si>
-    <t>12:34:54.766</t>
-  </si>
-  <si>
-    <t>12:35:10.699</t>
-  </si>
-  <si>
-    <t>12:35:36.418</t>
-  </si>
-  <si>
-    <t>12:36:01.318</t>
-  </si>
-  <si>
-    <t>12:36:13.122</t>
-  </si>
-  <si>
-    <t>12:36:16.027</t>
-  </si>
-  <si>
-    <t>12:36:12.652</t>
-  </si>
-  <si>
-    <t>12:36:26.822</t>
-  </si>
-  <si>
-    <t>12:36:11.887</t>
-  </si>
-  <si>
-    <t>12:36:34.188</t>
-  </si>
-  <si>
-    <t>12:36:11.156</t>
-  </si>
-  <si>
-    <t>12:36:35.552</t>
-  </si>
-  <si>
-    <t>12:36:10.592</t>
-  </si>
-  <si>
-    <t>12:36:42.796</t>
-  </si>
-  <si>
-    <t>12:35:35.449</t>
-  </si>
-  <si>
-    <t>12:36:44.482</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las transacciones del jugador PRAC06 del día lunes de customer maintenance aparecen exitosamente en pregame </t>
-  </si>
-  <si>
-    <t>12:36:54.303</t>
-  </si>
-  <si>
-    <t>12:36:55.050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El botón de  Iniciar Martes remueve las transacciones del día lunes del jugador PRAC06 existosamente  </t>
-  </si>
-  <si>
-    <t>12:36:59.957</t>
-  </si>
-  <si>
-    <t>12:37:12.396</t>
-  </si>
-  <si>
-    <t>12:36:55.897</t>
-  </si>
-  <si>
-    <t>12:37:17.789</t>
-  </si>
-  <si>
-    <t>13:09:32.965</t>
-  </si>
-  <si>
-    <t>13:09:58.171</t>
-  </si>
-  <si>
-    <t>13:10:10.005</t>
-  </si>
-  <si>
-    <t>13:10:12.895</t>
-  </si>
-  <si>
-    <t>13:10:09.581</t>
-  </si>
-  <si>
-    <t>13:10:23.290</t>
-  </si>
-  <si>
-    <t>13:10:08.823</t>
-  </si>
-  <si>
-    <t>13:10:30.463</t>
-  </si>
-  <si>
-    <t>13:10:08.066</t>
-  </si>
-  <si>
-    <t>13:10:31.727</t>
-  </si>
-  <si>
-    <t>13:10:07.395</t>
-  </si>
-  <si>
-    <t>13:10:39.796</t>
-  </si>
-  <si>
-    <t>13:09:32.042</t>
-  </si>
-  <si>
-    <t>13:10:41.538</t>
-  </si>
-  <si>
-    <t>13:10:51.499</t>
-  </si>
-  <si>
-    <t>13:10:52.306</t>
-  </si>
-  <si>
-    <t>13:11:02.003</t>
-  </si>
-  <si>
-    <t>13:11:14.982</t>
-  </si>
-  <si>
-    <t>13:10:53.073</t>
-  </si>
-  <si>
-    <t>13:11:27.958</t>
-  </si>
-  <si>
-    <t>13:13:13.809</t>
-  </si>
-  <si>
-    <t>13:13:52.440</t>
-  </si>
-  <si>
-    <t>13:17:40.153</t>
-  </si>
-  <si>
-    <t>13:18:04.457</t>
-  </si>
-  <si>
-    <t>13:17:39.172</t>
-  </si>
-  <si>
-    <t>13:18:09.523</t>
-  </si>
-  <si>
-    <t>13:19:59.134</t>
-  </si>
-  <si>
-    <t>13:20:25.105</t>
-  </si>
-  <si>
-    <t>13:19:58.218</t>
-  </si>
-  <si>
-    <t>13:21:01.320</t>
-  </si>
-  <si>
-    <t>13:23:18.615</t>
-  </si>
-  <si>
-    <t>13:23:43.399</t>
-  </si>
-  <si>
-    <t>13:23:17.825</t>
-  </si>
-  <si>
-    <t>13:24:19.716</t>
-  </si>
-  <si>
-    <t>13:28:53.499</t>
-  </si>
-  <si>
-    <t>13:29:21.160</t>
-  </si>
-  <si>
-    <t>13:28:51.632</t>
-  </si>
-  <si>
-    <t>13:29:29.308</t>
-  </si>
-  <si>
-    <t>13:32:40.976</t>
-  </si>
-  <si>
-    <t>13:33:06.535</t>
-  </si>
-  <si>
-    <t>13:32:39.911</t>
-  </si>
-  <si>
-    <t>13:33:12.292</t>
-  </si>
-  <si>
-    <t>La prueba no se pudo realizar debido a un fallo anomalo en la prueba Favor de revisar en la consola de katalon con el siguiente código -99</t>
-  </si>
-  <si>
-    <t>13:34:30.555</t>
-  </si>
-  <si>
-    <t>13:34:56.476</t>
-  </si>
-  <si>
-    <t>13:35:35.104</t>
-  </si>
-  <si>
-    <t>13:35:45.063</t>
-  </si>
-  <si>
-    <t>13:35:34.704</t>
-  </si>
-  <si>
-    <t>13:35:54.589</t>
-  </si>
-  <si>
-    <t>13:35:33.930</t>
-  </si>
-  <si>
-    <t>13:36:03.174</t>
-  </si>
-  <si>
-    <t>13:35:33.291</t>
-  </si>
-  <si>
-    <t>13:36:04.446</t>
-  </si>
-  <si>
-    <t>13:35:26.594</t>
-  </si>
-  <si>
-    <t>13:36:09.488</t>
-  </si>
-  <si>
-    <t>13:34:29.664</t>
-  </si>
-  <si>
-    <t>13:36:18.693</t>
-  </si>
-  <si>
-    <t>13:37:18.141</t>
-  </si>
-  <si>
-    <t>13:37:41.909</t>
-  </si>
-  <si>
-    <t>13:37:53.864</t>
-  </si>
-  <si>
-    <t>13:37:56.233</t>
-  </si>
-  <si>
-    <t>13:37:53.439</t>
-  </si>
-  <si>
-    <t>13:38:06.987</t>
-  </si>
-  <si>
-    <t>13:37:52.777</t>
-  </si>
-  <si>
-    <t>13:38:14.361</t>
-  </si>
-  <si>
-    <t>13:37:51.946</t>
-  </si>
-  <si>
-    <t>13:38:15.585</t>
-  </si>
-  <si>
-    <t>13:37:51.319</t>
-  </si>
-  <si>
-    <t>13:38:23.112</t>
-  </si>
-  <si>
-    <t>13:37:17.181</t>
-  </si>
-  <si>
-    <t>13:38:24.848</t>
-  </si>
-  <si>
-    <t>13:38:34.540</t>
-  </si>
-  <si>
-    <t>13:38:35.332</t>
-  </si>
-  <si>
-    <t>13:38:44.759</t>
-  </si>
-  <si>
-    <t>13:38:59.122</t>
-  </si>
-  <si>
-    <t>13:40:04.400</t>
-  </si>
-  <si>
-    <t>13:40:20.692</t>
-  </si>
-  <si>
-    <t>13:40:04.309</t>
-  </si>
-  <si>
-    <t>13:40:30.119</t>
-  </si>
-  <si>
-    <t>13:40:04.202</t>
-  </si>
-  <si>
-    <t>13:40:37.334</t>
-  </si>
-  <si>
-    <t>13:39:50.815</t>
-  </si>
-  <si>
-    <t>13:40:41.133</t>
-  </si>
-  <si>
-    <t>13:39:50.709</t>
-  </si>
-  <si>
-    <t>13:40:52.708</t>
-  </si>
-  <si>
-    <t>13:38:36.226</t>
-  </si>
-  <si>
-    <t>13:41:04.746</t>
+    <t>13:24:50.217</t>
+  </si>
+  <si>
+    <t>13:25:18.379</t>
+  </si>
+  <si>
+    <t>13:25:33.815</t>
+  </si>
+  <si>
+    <t>13:25:37.237</t>
+  </si>
+  <si>
+    <t>13:25:33.927</t>
+  </si>
+  <si>
+    <t>13:25:37.354</t>
+  </si>
+  <si>
+    <t>13:25:33.292</t>
+  </si>
+  <si>
+    <t>13:25:40.498</t>
+  </si>
+  <si>
+    <t>13:25:33.417</t>
+  </si>
+  <si>
+    <t>13:25:41.217</t>
+  </si>
+  <si>
+    <t>13:25:32.719</t>
+  </si>
+  <si>
+    <t>13:25:42.712</t>
+  </si>
+  <si>
+    <t>El jugador no logró ingresar al Overwiew debido a un paso de la prueba o elmento de la página que no está visible. Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  C6414-01</t>
+  </si>
+  <si>
+    <t>13:25:31.775</t>
+  </si>
+  <si>
+    <t>13:25:44.349</t>
+  </si>
+  <si>
+    <t>Validación de permiso Sportbook fallida  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  C3900-09</t>
+  </si>
+  <si>
+    <t>13:25:30.981</t>
+  </si>
+  <si>
+    <t>13:25:45.354</t>
+  </si>
+  <si>
+    <t>El botón de Balance Diario o Daily Figure de la sección "My Account"  no es visible debido a que un paso de la prueba no se completo o un elemento de la página que no está visible.  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>13:25:30.045</t>
+  </si>
+  <si>
+    <t>13:25:46.140</t>
+  </si>
+  <si>
+    <t>La tabla de días de la semana no muestra los días de la semana  debido a que un paso de la prueba no se completo o un elemento de la página que no está visible.  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09</t>
+  </si>
+  <si>
+    <t>13:24:45.613</t>
+  </si>
+  <si>
+    <t>13:25:46.940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugador PRAC06 no tiene transacciones para el día lunes o su configuración de zero balance no es del lunes o algún procedimiento previo como ingreso a pregame no se pudo completar  Para ver que elemento faltó, o que pasó no se cumplió, favor ir a la consola de katalon con el siguiente código  -09 o revisar el resultado de los siguientes casos de prueba [C6405, C6398] en el archivo excel de resultados de prueba para verificar si alguna precondición del caso de prueba falló </t>
+  </si>
+  <si>
+    <t>13:25:32.857</t>
+  </si>
+  <si>
+    <t>13:25:49.484</t>
+  </si>
+  <si>
+    <t>13:25:32.082</t>
+  </si>
+  <si>
+    <t>13:25:55.924</t>
+  </si>
+  <si>
+    <t>13:25:31.334</t>
+  </si>
+  <si>
+    <t>13:26:01.625</t>
+  </si>
+  <si>
+    <t>13:25:30.647</t>
+  </si>
+  <si>
+    <t>13:26:08.302</t>
+  </si>
+  <si>
+    <t>13:24:48.541</t>
+  </si>
+  <si>
+    <t>13:26:09.836</t>
+  </si>
+  <si>
+    <t>13:26:08.891</t>
+  </si>
+  <si>
+    <t>13:26:11.520</t>
+  </si>
+  <si>
+    <t>13:26:08.754</t>
+  </si>
+  <si>
+    <t>13:26:14.276</t>
+  </si>
+  <si>
+    <t>13:26:08.663</t>
+  </si>
+  <si>
+    <t>13:26:15.969</t>
+  </si>
+  <si>
+    <t>13:26:08.417</t>
+  </si>
+  <si>
+    <t>13:26:17.019</t>
+  </si>
+  <si>
+    <t>13:26:08.246</t>
+  </si>
+  <si>
+    <t>13:26:18.168</t>
+  </si>
+  <si>
+    <t>13:26:08.105</t>
+  </si>
+  <si>
+    <t>13:26:19.247</t>
+  </si>
+  <si>
+    <t>13:25:48.675</t>
+  </si>
+  <si>
+    <t>13:26:20.168</t>
+  </si>
+  <si>
+    <t>13:26:21.691</t>
+  </si>
+  <si>
+    <t>13:26:34.370</t>
+  </si>
+  <si>
+    <t>13:26:41.909</t>
+  </si>
+  <si>
+    <t>13:26:43.904</t>
+  </si>
+  <si>
+    <t>13:26:41.821</t>
+  </si>
+  <si>
+    <t>13:26:45.572</t>
+  </si>
+  <si>
+    <t>13:26:41.734</t>
+  </si>
+  <si>
+    <t>13:26:46.988</t>
+  </si>
+  <si>
+    <t>13:26:41.634</t>
+  </si>
+  <si>
+    <t>13:26:48.275</t>
+  </si>
+  <si>
+    <t>13:26:41.533</t>
+  </si>
+  <si>
+    <t>13:26:49.262</t>
+  </si>
+  <si>
+    <t>13:26:41.419</t>
+  </si>
+  <si>
+    <t>13:26:50.347</t>
+  </si>
+  <si>
+    <t>13:26:21.551</t>
+  </si>
+  <si>
+    <t>13:26:51.757</t>
+  </si>
+  <si>
+    <t>13:26:21.428</t>
+  </si>
+  <si>
+    <t>13:26:52.753</t>
+  </si>
+  <si>
+    <t>13:26:50.891</t>
+  </si>
+  <si>
+    <t>13:26:53.597</t>
+  </si>
+  <si>
+    <t>13:26:45.397</t>
+  </si>
+  <si>
+    <t>13:26:55.514</t>
+  </si>
+  <si>
+    <t>13:26:45.312</t>
+  </si>
+  <si>
+    <t>13:27:03.157</t>
+  </si>
+  <si>
+    <t>13:26:45.161</t>
+  </si>
+  <si>
+    <t>13:27:14.636</t>
+  </si>
+  <si>
+    <t>13:26:45.059</t>
+  </si>
+  <si>
+    <t>13:27:21.153</t>
+  </si>
+  <si>
+    <t>13:26:40.973</t>
+  </si>
+  <si>
+    <t>13:27:24.709</t>
+  </si>
+  <si>
+    <t>13:26:11.941</t>
+  </si>
+  <si>
+    <t>13:27:25.857</t>
+  </si>
+  <si>
+    <t>13:27:28.888</t>
+  </si>
+  <si>
+    <t>13:27:43.758</t>
+  </si>
+  <si>
+    <t>13:27:52.036</t>
+  </si>
+  <si>
+    <t>13:27:58.268</t>
+  </si>
+  <si>
+    <t>13:27:51.953</t>
+  </si>
+  <si>
+    <t>13:28:00.132</t>
+  </si>
+  <si>
+    <t>13:27:51.856</t>
+  </si>
+  <si>
+    <t>13:28:04.966</t>
+  </si>
+  <si>
+    <t>13:27:51.783</t>
+  </si>
+  <si>
+    <t>13:28:11.463</t>
+  </si>
+  <si>
+    <t>13:27:51.536</t>
+  </si>
+  <si>
+    <t>13:28:24.177</t>
+  </si>
+  <si>
+    <t>13:27:51.452</t>
+  </si>
+  <si>
+    <t>13:28:26.222</t>
+  </si>
+  <si>
+    <t>13:27:27.516</t>
+  </si>
+  <si>
+    <t>13:28:28.148</t>
+  </si>
+  <si>
+    <t>13:27:27.402</t>
+  </si>
+  <si>
+    <t>13:28:30.582</t>
+  </si>
+  <si>
+    <t>13:30:04.214</t>
+  </si>
+  <si>
+    <t>13:30:17.679</t>
+  </si>
+  <si>
+    <t>13:30:03.547</t>
+  </si>
+  <si>
+    <t>13:30:21.421</t>
+  </si>
+  <si>
+    <t>13:30:02.551</t>
+  </si>
+  <si>
+    <t>13:30:30.877</t>
+  </si>
+  <si>
+    <t>13:31:58.414</t>
+  </si>
+  <si>
+    <t>13:32:28.547</t>
+  </si>
+  <si>
+    <t>13:32:44.898</t>
+  </si>
+  <si>
+    <t>13:32:49.285</t>
+  </si>
+  <si>
+    <t>13:32:45.323</t>
+  </si>
+  <si>
+    <t>13:32:51.344</t>
+  </si>
+  <si>
+    <t>13:32:44.437</t>
+  </si>
+  <si>
+    <t>13:32:51.740</t>
+  </si>
+  <si>
+    <t>13:32:44.881</t>
+  </si>
+  <si>
+    <t>13:32:54.247</t>
+  </si>
+  <si>
+    <t>13:32:43.857</t>
+  </si>
+  <si>
+    <t>13:33:01.853</t>
+  </si>
+  <si>
+    <t>13:32:44.263</t>
+  </si>
+  <si>
+    <t>13:33:02.188</t>
+  </si>
+  <si>
+    <t>13:32:43.106</t>
+  </si>
+  <si>
+    <t>13:33:08.902</t>
+  </si>
+  <si>
+    <t>13:32:43.499</t>
+  </si>
+  <si>
+    <t>13:33:09.804</t>
+  </si>
+  <si>
+    <t>13:32:42.372</t>
+  </si>
+  <si>
+    <t>13:33:10.483</t>
+  </si>
+  <si>
+    <t>13:32:42.769</t>
+  </si>
+  <si>
+    <t>13:33:11.498</t>
+  </si>
+  <si>
+    <t>13:32:41.530</t>
+  </si>
+  <si>
+    <t>13:33:15.200</t>
+  </si>
+  <si>
+    <t>13:32:42.040</t>
+  </si>
+  <si>
+    <t>13:33:16.466</t>
+  </si>
+  <si>
+    <t>13:31:58.808</t>
+  </si>
+  <si>
+    <t>13:33:17.235</t>
+  </si>
+  <si>
+    <t>13:31:57.290</t>
+  </si>
+  <si>
+    <t>13:33:18.272</t>
+  </si>
+  <si>
+    <t>13:33:42.538</t>
+  </si>
+  <si>
+    <t>13:33:44.961</t>
+  </si>
+  <si>
+    <t>13:33:42.437</t>
+  </si>
+  <si>
+    <t>13:33:46.794</t>
+  </si>
+  <si>
+    <t>13:33:42.351</t>
+  </si>
+  <si>
+    <t>13:33:53.746</t>
+  </si>
+  <si>
+    <t>13:33:42.247</t>
+  </si>
+  <si>
+    <t>13:34:00.880</t>
+  </si>
+  <si>
+    <t>13:33:42.137</t>
+  </si>
+  <si>
+    <t>13:34:02.122</t>
+  </si>
+  <si>
+    <t>13:33:42.038</t>
+  </si>
+  <si>
+    <t>13:34:05.796</t>
+  </si>
+  <si>
+    <t>13:33:18.972</t>
+  </si>
+  <si>
+    <t>13:34:09.689</t>
+  </si>
+  <si>
+    <t>13:34:17.805</t>
+  </si>
+  <si>
+    <t>13:34:20.212</t>
+  </si>
+  <si>
+    <t>13:34:10.654</t>
+  </si>
+  <si>
+    <t>13:34:25.015</t>
+  </si>
+  <si>
+    <t>13:34:11.115</t>
+  </si>
+  <si>
+    <t>13:34:25.883</t>
+  </si>
+  <si>
+    <t>13:34:11.018</t>
+  </si>
+  <si>
+    <t>13:34:33.273</t>
+  </si>
+  <si>
+    <t>13:34:33.971</t>
+  </si>
+  <si>
+    <t>13:34:36.446</t>
+  </si>
+  <si>
+    <t>13:34:33.817</t>
+  </si>
+  <si>
+    <t>13:34:38.064</t>
+  </si>
+  <si>
+    <t>13:34:10.912</t>
+  </si>
+  <si>
+    <t>13:34:40.523</t>
+  </si>
+  <si>
+    <t>13:34:10.801</t>
+  </si>
+  <si>
+    <t>13:34:42.280</t>
+  </si>
+  <si>
+    <t>13:34:33.731</t>
+  </si>
+  <si>
+    <t>13:34:45.105</t>
+  </si>
+  <si>
+    <t>13:34:04.624</t>
+  </si>
+  <si>
+    <t>13:34:46.415</t>
+  </si>
+  <si>
+    <t>13:33:17.982</t>
+  </si>
+  <si>
+    <t>13:34:50.776</t>
+  </si>
+  <si>
+    <t>13:34:33.618</t>
+  </si>
+  <si>
+    <t>13:34:52.307</t>
+  </si>
+  <si>
+    <t>13:34:33.502</t>
+  </si>
+  <si>
+    <t>13:34:53.544</t>
+  </si>
+  <si>
+    <t>13:34:33.345</t>
+  </si>
+  <si>
+    <t>13:34:57.420</t>
+  </si>
+  <si>
+    <t>13:34:10.523</t>
+  </si>
+  <si>
+    <t>13:34:58.773</t>
+  </si>
+  <si>
+    <t>13:34:10.422</t>
+  </si>
+  <si>
+    <t>13:34:59.615</t>
+  </si>
+  <si>
+    <t>13:34:57.076</t>
+  </si>
+  <si>
+    <t>13:35:18.916</t>
+  </si>
+  <si>
+    <t>13:35:33.433</t>
+  </si>
+  <si>
+    <t>13:35:41.393</t>
+  </si>
+  <si>
+    <t>13:35:33.348</t>
+  </si>
+  <si>
+    <t>13:35:43.058</t>
+  </si>
+  <si>
+    <t>13:35:33.262</t>
+  </si>
+  <si>
+    <t>13:35:53.108</t>
+  </si>
+  <si>
+    <t>13:35:33.167</t>
+  </si>
+  <si>
+    <t>13:36:00.151</t>
+  </si>
+  <si>
+    <t>13:35:32.300</t>
+  </si>
+  <si>
+    <t>13:36:01.340</t>
+  </si>
+  <si>
+    <t>13:35:27.030</t>
+  </si>
+  <si>
+    <t>13:36:04.957</t>
+  </si>
+  <si>
+    <t>13:34:56.973</t>
+  </si>
+  <si>
+    <t>13:36:06.399</t>
+  </si>
+  <si>
+    <t>13:34:56.869</t>
+  </si>
+  <si>
+    <t>13:36:08.259</t>
+  </si>
+  <si>
+    <t>13:42:08.801</t>
+  </si>
+  <si>
+    <t>13:42:37.950</t>
+  </si>
+  <si>
+    <t>13:42:54.498</t>
+  </si>
+  <si>
+    <t>13:42:58.188</t>
+  </si>
+  <si>
+    <t>13:42:54.952</t>
+  </si>
+  <si>
+    <t>13:42:59.010</t>
+  </si>
+  <si>
+    <t>13:42:53.621</t>
+  </si>
+  <si>
+    <t>13:43:02.525</t>
+  </si>
+  <si>
+    <t>13:42:54.483</t>
+  </si>
+  <si>
+    <t>13:43:02.780</t>
+  </si>
+  <si>
+    <t>13:42:53.260</t>
+  </si>
+  <si>
+    <t>13:43:11.290</t>
+  </si>
+  <si>
+    <t>13:42:52.997</t>
+  </si>
+  <si>
+    <t>13:43:11.823</t>
+  </si>
+  <si>
+    <t>13:42:52.421</t>
+  </si>
+  <si>
+    <t>13:43:18.471</t>
+  </si>
+  <si>
+    <t>13:42:52.105</t>
+  </si>
+  <si>
+    <t>13:43:19.501</t>
+  </si>
+  <si>
+    <t>13:42:51.635</t>
+  </si>
+  <si>
+    <t>13:43:20.407</t>
+  </si>
+  <si>
+    <t>13:42:51.346</t>
+  </si>
+  <si>
+    <t>13:43:21.256</t>
+  </si>
+  <si>
+    <t>13:42:50.707</t>
+  </si>
+  <si>
+    <t>13:43:25.158</t>
+  </si>
+  <si>
+    <t>13:42:50.624</t>
+  </si>
+  <si>
+    <t>13:43:26.432</t>
+  </si>
+  <si>
+    <t>13:42:06.704</t>
+  </si>
+  <si>
+    <t>13:43:27.595</t>
+  </si>
+  <si>
+    <t>13:42:06.761</t>
+  </si>
+  <si>
+    <t>13:43:28.793</t>
   </si>
 </sst>
 </file>
@@ -1587,25 +2080,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>357</v>
+        <v>512</v>
       </c>
       <c r="F2" t="s">
-        <v>358</v>
+        <v>513</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1673,25 +2166,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>217</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>218</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -1758,19 +2251,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1851,22 +2344,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1881,7 +2374,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1943,22 +2436,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1973,7 +2466,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2040,25 +2533,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>359</v>
+        <v>516</v>
       </c>
       <c r="F2" t="s">
-        <v>360</v>
+        <v>517</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2067,7 +2560,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2129,19 +2622,19 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>355</v>
+        <v>504</v>
       </c>
       <c r="D2" t="s">
-        <v>356</v>
+        <v>505</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -2150,7 +2643,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>155</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2162,9 +2655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2202,22 +2693,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>215</v>
+        <v>508</v>
       </c>
       <c r="D2" t="s">
-        <v>216</v>
+        <v>509</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -2226,7 +2717,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>158</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2239,7 +2730,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,22 +2778,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2317,7 +2808,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2407,22 +2898,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2437,7 +2928,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2495,19 +2986,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2522,7 +3013,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2592,25 +3083,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>199</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2674,22 +3165,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -2704,7 +3195,7 @@
         <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2717,7 +3208,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2762,25 +3253,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>361</v>
+        <v>520</v>
       </c>
       <c r="F2" t="s">
-        <v>362</v>
+        <v>521</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2789,7 +3280,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2855,25 +3346,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2882,7 +3373,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2940,25 +3431,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>363</v>
+        <v>524</v>
       </c>
       <c r="F2" t="s">
-        <v>364</v>
+        <v>525</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -2967,7 +3458,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3025,28 +3516,28 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3055,7 +3546,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3113,25 +3604,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
+        <v>260</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>261</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>251</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3140,7 +3631,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -3153,7 +3644,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3198,25 +3689,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>349</v>
+        <v>528</v>
       </c>
       <c r="F2" t="s">
-        <v>350</v>
+        <v>529</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3225,7 +3716,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>272</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3283,19 +3774,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -3310,7 +3801,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3368,25 +3859,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>365</v>
+        <v>470</v>
       </c>
       <c r="F2" t="s">
-        <v>366</v>
+        <v>471</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3395,7 +3886,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3447,25 +3938,25 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
         <v>103</v>
       </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
-        <v>353</v>
+        <v>500</v>
       </c>
       <c r="E2" t="s">
-        <v>354</v>
+        <v>501</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -3474,7 +3965,7 @@
         <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>221</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3486,8 +3977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3551,19 +4042,19 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>187</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>188</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3572,7 +4063,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
@@ -3633,25 +4124,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>351</v>
+        <v>498</v>
       </c>
       <c r="F2" t="s">
-        <v>352</v>
+        <v>499</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3660,7 +4151,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>275</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3673,7 +4164,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3715,37 +4206,37 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
         <v>103</v>
-      </c>
-      <c r="B2" t="s">
-        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3754,11 +4245,11 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229C7116-4E07-47F6-B6A2-AA3E67FD8174}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830D8FEC-E448-46DD-958F-4AC130B4257C}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3800,34 +4291,37 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>103</v>
       </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>245</v>
       </c>
       <c r="F2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>97</v>
-      </c>
       <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
-        <v>121</v>
+      <c r="K2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3836,11 +4330,95 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830D8FEC-E448-46DD-958F-4AC130B4257C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A67EC6-55E7-4CF8-9B31-FEC85A3ED160}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{954D9941-CAC5-43FB-91FB-1233CCBE2338}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3885,34 +4463,34 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="F2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3920,12 +4498,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{425D959C-196F-4131-A78D-F0B10FB4A717}">
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEA98F0-9128-4583-B476-4D3E6ABA39A7}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3970,25 +4548,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -3997,7 +4575,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -4005,12 +4583,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BA8E2D-405E-4E0A-8CFA-9B3F41877BEE}">
-  <dimension ref="A1:K2"/>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D089B1A-DE1B-4B6F-8D13-C980710CB4B0}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4050,30 +4628,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>262</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>263</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>251</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -4082,10 +4660,192 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>140</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF0E11B-A4F4-4BFC-BA93-0BE0BA56E645}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A358977F-F3AA-4EDA-9F1D-E8325A09020C}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEBACE7-0CA6-4465-8492-5C3AED7A31A0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4143,37 +4903,37 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>181</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>182</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -4236,19 +4996,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -4325,25 +5085,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>205</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -4410,25 +5170,25 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>212</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -4503,19 +5263,19 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>193</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>194</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -4576,13 +5336,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>

</xml_diff>